<commit_message>
Added new values to OBInternalStatementFeeType1Code
Added UK.OBIE.InstalmentPlan and  UK.OBIE.ReturnedPayment to OBInternalStatementFeeType1Code
</commit_message>
<xml_diff>
--- a/OB_Internal_Codeset.xlsx
+++ b/OB_Internal_Codeset.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chris/OpenBanking/GitHub/External_Internal_CodeSets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/GitHub-repos/External_Internal_CodeSets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{02BBC9B6-D84C-8944-B8FF-46CF8B9E42A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{074894BE-1596-9E4C-888B-8DF0AFA996E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="620" windowWidth="38400" windowHeight="19820" xr2:uid="{4BA74A73-F883-C94E-AE65-527FEAB24FBE}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="34560" windowHeight="19820" xr2:uid="{4BA74A73-F883-C94E-AE65-527FEAB24FBE}"/>
   </bookViews>
   <sheets>
     <sheet name="OB_Internal_Codeset" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2834" uniqueCount="1797">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2842" uniqueCount="1801">
   <si>
     <t>Code Set</t>
   </si>
@@ -5490,6 +5490,18 @@
   </si>
   <si>
     <t>Urgent</t>
+  </si>
+  <si>
+    <t>UK.OBIE.InstalmentPlan</t>
+  </si>
+  <si>
+    <t>Instalment plan fees charged during the statement period.</t>
+  </si>
+  <si>
+    <t>UK.OBIE.ReturnedPayment</t>
+  </si>
+  <si>
+    <t>Returned payment fees charged during the statement period.</t>
   </si>
 </sst>
 </file>
@@ -6048,13 +6060,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FFFB267F-52FF-2549-863C-D165F57A28C3}" name="Table1" displayName="Table1" ref="A1:F712" totalsRowShown="0">
-  <autoFilter ref="A1:F712" xr:uid="{FFFB267F-52FF-2549-863C-D165F57A28C3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FFFB267F-52FF-2549-863C-D165F57A28C3}" name="Table1" displayName="Table1" ref="A1:F714" totalsRowShown="0">
+  <autoFilter ref="A1:F714" xr:uid="{FFFB267F-52FF-2549-863C-D165F57A28C3}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{23F53907-045A-2545-8FDE-B8095E843B7C}" name="Code Set"/>
     <tableColumn id="2" xr3:uid="{8D12A497-C96F-094C-9D20-C8F6648FDFDB}" name="Code Value"/>
-    <tableColumn id="3" xr3:uid="{B15DCD15-9901-8B4A-BD58-10A8176811D3}" name="Code Name" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{0CCBD569-51CF-F844-B255-57C54AE66C0A}" name="Code Definition" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{B15DCD15-9901-8B4A-BD58-10A8176811D3}" name="Code Name" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{0CCBD569-51CF-F844-B255-57C54AE66C0A}" name="Code Definition" dataDxfId="1"/>
     <tableColumn id="5" xr3:uid="{8C9D593D-81B6-8B41-AB4B-AE966120D2A3}" name="HTTP Status Category"/>
     <tableColumn id="6" xr3:uid="{5C309560-0FAB-CB4C-85E8-B6E9C1DB29EB}" name="Description" dataDxfId="0"/>
   </tableColumns>
@@ -6379,10 +6391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EB901B9-ECA3-B946-8761-40B7A833F7F4}">
-  <dimension ref="A1:F712"/>
+  <dimension ref="A1:F714"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A656" workbookViewId="0">
-      <selection activeCell="D87" sqref="D87"/>
+    <sheetView tabSelected="1" topLeftCell="A481" workbookViewId="0">
+      <selection activeCell="A486" sqref="A486"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11342,7 +11354,7 @@
         <v>973</v>
       </c>
     </row>
-    <row r="349" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A349" t="s">
         <v>6</v>
       </c>
@@ -11762,7 +11774,7 @@
         <v>1063</v>
       </c>
     </row>
-    <row r="379" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="379" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A379" t="s">
         <v>6</v>
       </c>
@@ -13556,30 +13568,30 @@
     </row>
     <row r="507" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A507" t="s">
-        <v>1395</v>
+        <v>1364</v>
       </c>
       <c r="B507" t="s">
-        <v>1367</v>
+        <v>1797</v>
       </c>
       <c r="C507" s="1" t="s">
-        <v>1367</v>
+        <v>1797</v>
       </c>
       <c r="D507" s="1" t="s">
-        <v>1396</v>
+        <v>1798</v>
       </c>
     </row>
     <row r="508" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A508" t="s">
-        <v>1395</v>
+        <v>1364</v>
       </c>
       <c r="B508" t="s">
-        <v>1397</v>
+        <v>1799</v>
       </c>
       <c r="C508" s="1" t="s">
-        <v>1397</v>
+        <v>1799</v>
       </c>
       <c r="D508" s="1" t="s">
-        <v>1398</v>
+        <v>1800</v>
       </c>
     </row>
     <row r="509" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -13587,13 +13599,13 @@
         <v>1395</v>
       </c>
       <c r="B509" t="s">
-        <v>1399</v>
+        <v>1367</v>
       </c>
       <c r="C509" s="1" t="s">
-        <v>1399</v>
+        <v>1367</v>
       </c>
       <c r="D509" s="1" t="s">
-        <v>1400</v>
+        <v>1396</v>
       </c>
     </row>
     <row r="510" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -13601,13 +13613,13 @@
         <v>1395</v>
       </c>
       <c r="B510" t="s">
-        <v>1401</v>
+        <v>1397</v>
       </c>
       <c r="C510" s="1" t="s">
-        <v>1401</v>
+        <v>1397</v>
       </c>
       <c r="D510" s="1" t="s">
-        <v>1402</v>
+        <v>1398</v>
       </c>
     </row>
     <row r="511" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -13615,41 +13627,41 @@
         <v>1395</v>
       </c>
       <c r="B511" t="s">
-        <v>1393</v>
+        <v>1399</v>
       </c>
       <c r="C511" s="1" t="s">
-        <v>1393</v>
+        <v>1399</v>
       </c>
       <c r="D511" s="1" t="s">
-        <v>1403</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="512" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A512" t="s">
-        <v>1404</v>
+        <v>1395</v>
       </c>
       <c r="B512" t="s">
-        <v>1405</v>
+        <v>1401</v>
       </c>
       <c r="C512" s="1" t="s">
-        <v>1405</v>
+        <v>1401</v>
       </c>
       <c r="D512" s="1" t="s">
-        <v>1406</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="513" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A513" t="s">
-        <v>1404</v>
+        <v>1395</v>
       </c>
       <c r="B513" t="s">
-        <v>1407</v>
+        <v>1393</v>
       </c>
       <c r="C513" s="1" t="s">
-        <v>1407</v>
+        <v>1393</v>
       </c>
       <c r="D513" s="1" t="s">
-        <v>1408</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="514" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -13657,13 +13669,13 @@
         <v>1404</v>
       </c>
       <c r="B514" t="s">
-        <v>1409</v>
+        <v>1405</v>
       </c>
       <c r="C514" s="1" t="s">
-        <v>1409</v>
+        <v>1405</v>
       </c>
       <c r="D514" s="1" t="s">
-        <v>1410</v>
+        <v>1406</v>
       </c>
     </row>
     <row r="515" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -13671,13 +13683,13 @@
         <v>1404</v>
       </c>
       <c r="B515" t="s">
-        <v>1411</v>
+        <v>1407</v>
       </c>
       <c r="C515" s="1" t="s">
-        <v>1411</v>
+        <v>1407</v>
       </c>
       <c r="D515" s="1" t="s">
-        <v>1412</v>
+        <v>1408</v>
       </c>
     </row>
     <row r="516" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -13685,13 +13697,13 @@
         <v>1404</v>
       </c>
       <c r="B516" t="s">
-        <v>1413</v>
+        <v>1409</v>
       </c>
       <c r="C516" s="1" t="s">
-        <v>1413</v>
+        <v>1409</v>
       </c>
       <c r="D516" s="1" t="s">
-        <v>1414</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="517" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -13699,13 +13711,13 @@
         <v>1404</v>
       </c>
       <c r="B517" t="s">
-        <v>1415</v>
+        <v>1411</v>
       </c>
       <c r="C517" s="1" t="s">
-        <v>1415</v>
+        <v>1411</v>
       </c>
       <c r="D517" s="1" t="s">
-        <v>1416</v>
+        <v>1412</v>
       </c>
     </row>
     <row r="518" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -13713,13 +13725,13 @@
         <v>1404</v>
       </c>
       <c r="B518" t="s">
-        <v>1417</v>
+        <v>1413</v>
       </c>
       <c r="C518" s="1" t="s">
-        <v>1417</v>
+        <v>1413</v>
       </c>
       <c r="D518" s="1" t="s">
-        <v>1418</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="519" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -13727,13 +13739,13 @@
         <v>1404</v>
       </c>
       <c r="B519" t="s">
-        <v>1419</v>
+        <v>1415</v>
       </c>
       <c r="C519" s="1" t="s">
-        <v>1419</v>
+        <v>1415</v>
       </c>
       <c r="D519" s="1" t="s">
-        <v>1420</v>
+        <v>1416</v>
       </c>
     </row>
     <row r="520" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -13741,13 +13753,13 @@
         <v>1404</v>
       </c>
       <c r="B520" t="s">
-        <v>1421</v>
+        <v>1417</v>
       </c>
       <c r="C520" s="1" t="s">
-        <v>1421</v>
+        <v>1417</v>
       </c>
       <c r="D520" s="1" t="s">
-        <v>1422</v>
+        <v>1418</v>
       </c>
     </row>
     <row r="521" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -13755,41 +13767,41 @@
         <v>1404</v>
       </c>
       <c r="B521" t="s">
-        <v>1423</v>
+        <v>1419</v>
       </c>
       <c r="C521" s="1" t="s">
-        <v>1423</v>
+        <v>1419</v>
       </c>
       <c r="D521" s="1" t="s">
-        <v>1424</v>
+        <v>1420</v>
       </c>
     </row>
     <row r="522" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A522" t="s">
-        <v>1425</v>
+        <v>1404</v>
       </c>
       <c r="B522" t="s">
-        <v>1426</v>
+        <v>1421</v>
       </c>
       <c r="C522" s="1" t="s">
-        <v>1426</v>
+        <v>1421</v>
       </c>
       <c r="D522" s="1" t="s">
-        <v>1427</v>
+        <v>1422</v>
       </c>
     </row>
     <row r="523" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A523" t="s">
-        <v>1425</v>
+        <v>1404</v>
       </c>
       <c r="B523" t="s">
-        <v>1428</v>
+        <v>1423</v>
       </c>
       <c r="C523" s="1" t="s">
-        <v>1428</v>
+        <v>1423</v>
       </c>
       <c r="D523" s="1" t="s">
-        <v>1427</v>
+        <v>1424</v>
       </c>
     </row>
     <row r="524" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -13797,13 +13809,13 @@
         <v>1425</v>
       </c>
       <c r="B524" t="s">
-        <v>1429</v>
+        <v>1426</v>
       </c>
       <c r="C524" s="1" t="s">
-        <v>1429</v>
+        <v>1426</v>
       </c>
       <c r="D524" s="1" t="s">
-        <v>1430</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="525" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -13811,13 +13823,13 @@
         <v>1425</v>
       </c>
       <c r="B525" t="s">
-        <v>1431</v>
+        <v>1428</v>
       </c>
       <c r="C525" s="1" t="s">
-        <v>1431</v>
+        <v>1428</v>
       </c>
       <c r="D525" s="1" t="s">
-        <v>1432</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="526" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -13825,13 +13837,13 @@
         <v>1425</v>
       </c>
       <c r="B526" t="s">
-        <v>1433</v>
+        <v>1429</v>
       </c>
       <c r="C526" s="1" t="s">
-        <v>1433</v>
+        <v>1429</v>
       </c>
       <c r="D526" s="1" t="s">
-        <v>1434</v>
+        <v>1430</v>
       </c>
     </row>
     <row r="527" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -13839,13 +13851,13 @@
         <v>1425</v>
       </c>
       <c r="B527" t="s">
-        <v>1435</v>
+        <v>1431</v>
       </c>
       <c r="C527" s="1" t="s">
-        <v>1435</v>
+        <v>1431</v>
       </c>
       <c r="D527" s="1" t="s">
-        <v>1434</v>
+        <v>1432</v>
       </c>
     </row>
     <row r="528" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -13853,13 +13865,13 @@
         <v>1425</v>
       </c>
       <c r="B528" t="s">
-        <v>1436</v>
+        <v>1433</v>
       </c>
       <c r="C528" s="1" t="s">
-        <v>1436</v>
+        <v>1433</v>
       </c>
       <c r="D528" s="1" t="s">
-        <v>1437</v>
+        <v>1434</v>
       </c>
     </row>
     <row r="529" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -13867,69 +13879,69 @@
         <v>1425</v>
       </c>
       <c r="B529" t="s">
-        <v>1438</v>
+        <v>1435</v>
       </c>
       <c r="C529" s="1" t="s">
-        <v>1438</v>
+        <v>1435</v>
       </c>
       <c r="D529" s="1" t="s">
+        <v>1434</v>
+      </c>
+    </row>
+    <row r="530" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A530" t="s">
+        <v>1425</v>
+      </c>
+      <c r="B530" t="s">
+        <v>1436</v>
+      </c>
+      <c r="C530" s="1" t="s">
+        <v>1436</v>
+      </c>
+      <c r="D530" s="1" t="s">
         <v>1437</v>
-      </c>
-    </row>
-    <row r="530" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A530" t="s">
-        <v>1439</v>
-      </c>
-      <c r="B530" t="s">
-        <v>1440</v>
-      </c>
-      <c r="C530" s="1" t="s">
-        <v>1440</v>
-      </c>
-      <c r="D530" s="1" t="s">
-        <v>1441</v>
       </c>
     </row>
     <row r="531" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A531" t="s">
+        <v>1425</v>
+      </c>
+      <c r="B531" t="s">
+        <v>1438</v>
+      </c>
+      <c r="C531" s="1" t="s">
+        <v>1438</v>
+      </c>
+      <c r="D531" s="1" t="s">
+        <v>1437</v>
+      </c>
+    </row>
+    <row r="532" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A532" t="s">
         <v>1439</v>
       </c>
-      <c r="B531" t="s">
+      <c r="B532" t="s">
+        <v>1440</v>
+      </c>
+      <c r="C532" s="1" t="s">
+        <v>1440</v>
+      </c>
+      <c r="D532" s="1" t="s">
+        <v>1441</v>
+      </c>
+    </row>
+    <row r="533" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A533" t="s">
+        <v>1439</v>
+      </c>
+      <c r="B533" t="s">
         <v>1442</v>
       </c>
-      <c r="C531" s="1" t="s">
+      <c r="C533" s="1" t="s">
         <v>1442</v>
       </c>
-      <c r="D531" s="1" t="s">
+      <c r="D533" s="1" t="s">
         <v>1443</v>
-      </c>
-    </row>
-    <row r="532" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A532" t="s">
-        <v>1444</v>
-      </c>
-      <c r="B532" t="s">
-        <v>1445</v>
-      </c>
-      <c r="C532" s="1" t="s">
-        <v>1445</v>
-      </c>
-      <c r="D532" s="1" t="s">
-        <v>1446</v>
-      </c>
-    </row>
-    <row r="533" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A533" t="s">
-        <v>1444</v>
-      </c>
-      <c r="B533" t="s">
-        <v>1447</v>
-      </c>
-      <c r="C533" s="1" t="s">
-        <v>1447</v>
-      </c>
-      <c r="D533" s="1" t="s">
-        <v>1448</v>
       </c>
     </row>
     <row r="534" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -13937,13 +13949,13 @@
         <v>1444</v>
       </c>
       <c r="B534" t="s">
-        <v>1449</v>
+        <v>1445</v>
       </c>
       <c r="C534" s="1" t="s">
-        <v>1449</v>
+        <v>1445</v>
       </c>
       <c r="D534" s="1" t="s">
-        <v>1450</v>
+        <v>1446</v>
       </c>
     </row>
     <row r="535" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -13951,13 +13963,13 @@
         <v>1444</v>
       </c>
       <c r="B535" t="s">
-        <v>1451</v>
+        <v>1447</v>
       </c>
       <c r="C535" s="1" t="s">
-        <v>1451</v>
+        <v>1447</v>
       </c>
       <c r="D535" s="1" t="s">
-        <v>1452</v>
+        <v>1448</v>
       </c>
     </row>
     <row r="536" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -13965,13 +13977,13 @@
         <v>1444</v>
       </c>
       <c r="B536" t="s">
-        <v>1453</v>
+        <v>1449</v>
       </c>
       <c r="C536" s="1" t="s">
-        <v>1453</v>
+        <v>1449</v>
       </c>
       <c r="D536" s="1" t="s">
-        <v>1454</v>
+        <v>1450</v>
       </c>
     </row>
     <row r="537" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -13979,55 +13991,55 @@
         <v>1444</v>
       </c>
       <c r="B537" t="s">
-        <v>1455</v>
+        <v>1451</v>
       </c>
       <c r="C537" s="1" t="s">
-        <v>1455</v>
+        <v>1451</v>
       </c>
       <c r="D537" s="1" t="s">
-        <v>1456</v>
-      </c>
-    </row>
-    <row r="538" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>1452</v>
+      </c>
+    </row>
+    <row r="538" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A538" t="s">
-        <v>1457</v>
+        <v>1444</v>
       </c>
       <c r="B538" t="s">
-        <v>1458</v>
+        <v>1453</v>
       </c>
       <c r="C538" s="1" t="s">
-        <v>1458</v>
+        <v>1453</v>
       </c>
       <c r="D538" s="1" t="s">
-        <v>1459</v>
+        <v>1454</v>
       </c>
     </row>
     <row r="539" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A539" t="s">
-        <v>1457</v>
+        <v>1444</v>
       </c>
       <c r="B539" t="s">
-        <v>1460</v>
+        <v>1455</v>
       </c>
       <c r="C539" s="1" t="s">
-        <v>1460</v>
+        <v>1455</v>
       </c>
       <c r="D539" s="1" t="s">
-        <v>1461</v>
-      </c>
-    </row>
-    <row r="540" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>1456</v>
+      </c>
+    </row>
+    <row r="540" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A540" t="s">
         <v>1457</v>
       </c>
       <c r="B540" t="s">
-        <v>1462</v>
+        <v>1458</v>
       </c>
       <c r="C540" s="1" t="s">
-        <v>1462</v>
+        <v>1458</v>
       </c>
       <c r="D540" s="1" t="s">
-        <v>1463</v>
+        <v>1459</v>
       </c>
     </row>
     <row r="541" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14035,13 +14047,13 @@
         <v>1457</v>
       </c>
       <c r="B541" t="s">
-        <v>1464</v>
+        <v>1460</v>
       </c>
       <c r="C541" s="1" t="s">
-        <v>1464</v>
+        <v>1460</v>
       </c>
       <c r="D541" s="1" t="s">
-        <v>1465</v>
+        <v>1461</v>
       </c>
     </row>
     <row r="542" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14049,41 +14061,41 @@
         <v>1457</v>
       </c>
       <c r="B542" t="s">
-        <v>1466</v>
+        <v>1462</v>
       </c>
       <c r="C542" s="1" t="s">
-        <v>1466</v>
+        <v>1462</v>
       </c>
       <c r="D542" s="1" t="s">
-        <v>1467</v>
+        <v>1463</v>
       </c>
     </row>
     <row r="543" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A543" t="s">
-        <v>1468</v>
+        <v>1457</v>
       </c>
       <c r="B543" t="s">
-        <v>1469</v>
+        <v>1464</v>
       </c>
       <c r="C543" s="1" t="s">
-        <v>1469</v>
+        <v>1464</v>
       </c>
       <c r="D543" s="1" t="s">
-        <v>1470</v>
+        <v>1465</v>
       </c>
     </row>
     <row r="544" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A544" t="s">
-        <v>1468</v>
+        <v>1457</v>
       </c>
       <c r="B544" t="s">
-        <v>1471</v>
+        <v>1466</v>
       </c>
       <c r="C544" s="1" t="s">
-        <v>1471</v>
+        <v>1466</v>
       </c>
       <c r="D544" s="1" t="s">
-        <v>1472</v>
+        <v>1467</v>
       </c>
     </row>
     <row r="545" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14091,13 +14103,13 @@
         <v>1468</v>
       </c>
       <c r="B545" t="s">
-        <v>1383</v>
+        <v>1469</v>
       </c>
       <c r="C545" s="1" t="s">
-        <v>1383</v>
+        <v>1469</v>
       </c>
       <c r="D545" s="1" t="s">
-        <v>1473</v>
+        <v>1470</v>
       </c>
     </row>
     <row r="546" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14105,13 +14117,13 @@
         <v>1468</v>
       </c>
       <c r="B546" t="s">
-        <v>1474</v>
+        <v>1471</v>
       </c>
       <c r="C546" s="1" t="s">
-        <v>1474</v>
+        <v>1471</v>
       </c>
       <c r="D546" s="1" t="s">
-        <v>1475</v>
+        <v>1472</v>
       </c>
     </row>
     <row r="547" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14119,13 +14131,13 @@
         <v>1468</v>
       </c>
       <c r="B547" t="s">
-        <v>1453</v>
+        <v>1383</v>
       </c>
       <c r="C547" s="1" t="s">
-        <v>1453</v>
+        <v>1383</v>
       </c>
       <c r="D547" s="1" t="s">
-        <v>1454</v>
+        <v>1473</v>
       </c>
     </row>
     <row r="548" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14133,13 +14145,13 @@
         <v>1468</v>
       </c>
       <c r="B548" t="s">
-        <v>1455</v>
+        <v>1474</v>
       </c>
       <c r="C548" s="1" t="s">
-        <v>1455</v>
+        <v>1474</v>
       </c>
       <c r="D548" s="1" t="s">
-        <v>1456</v>
+        <v>1475</v>
       </c>
     </row>
     <row r="549" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14147,41 +14159,41 @@
         <v>1468</v>
       </c>
       <c r="B549" t="s">
-        <v>1476</v>
+        <v>1453</v>
       </c>
       <c r="C549" s="1" t="s">
-        <v>1476</v>
+        <v>1453</v>
       </c>
       <c r="D549" s="1" t="s">
-        <v>1477</v>
+        <v>1454</v>
       </c>
     </row>
     <row r="550" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A550" t="s">
-        <v>1478</v>
+        <v>1468</v>
       </c>
       <c r="B550" t="s">
-        <v>1479</v>
+        <v>1455</v>
       </c>
       <c r="C550" s="1" t="s">
-        <v>1479</v>
+        <v>1455</v>
       </c>
       <c r="D550" s="1" t="s">
-        <v>1480</v>
+        <v>1456</v>
       </c>
     </row>
     <row r="551" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A551" t="s">
-        <v>1478</v>
+        <v>1468</v>
       </c>
       <c r="B551" t="s">
-        <v>1481</v>
+        <v>1476</v>
       </c>
       <c r="C551" s="1" t="s">
-        <v>1481</v>
+        <v>1476</v>
       </c>
       <c r="D551" s="1" t="s">
-        <v>1482</v>
+        <v>1477</v>
       </c>
     </row>
     <row r="552" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14189,13 +14201,13 @@
         <v>1478</v>
       </c>
       <c r="B552" t="s">
-        <v>1483</v>
+        <v>1479</v>
       </c>
       <c r="C552" s="1" t="s">
-        <v>1483</v>
+        <v>1479</v>
       </c>
       <c r="D552" s="1" t="s">
-        <v>1484</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="553" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14203,13 +14215,13 @@
         <v>1478</v>
       </c>
       <c r="B553" t="s">
-        <v>1485</v>
+        <v>1481</v>
       </c>
       <c r="C553" s="1" t="s">
-        <v>1485</v>
+        <v>1481</v>
       </c>
       <c r="D553" s="1" t="s">
-        <v>1486</v>
+        <v>1482</v>
       </c>
     </row>
     <row r="554" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14217,13 +14229,13 @@
         <v>1478</v>
       </c>
       <c r="B554" t="s">
-        <v>1487</v>
+        <v>1483</v>
       </c>
       <c r="C554" s="1" t="s">
-        <v>1487</v>
+        <v>1483</v>
       </c>
       <c r="D554" s="1" t="s">
-        <v>1488</v>
+        <v>1484</v>
       </c>
     </row>
     <row r="555" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14231,13 +14243,13 @@
         <v>1478</v>
       </c>
       <c r="B555" t="s">
-        <v>1489</v>
+        <v>1485</v>
       </c>
       <c r="C555" s="1" t="s">
-        <v>1489</v>
+        <v>1485</v>
       </c>
       <c r="D555" s="1" t="s">
-        <v>1490</v>
+        <v>1486</v>
       </c>
     </row>
     <row r="556" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14245,13 +14257,13 @@
         <v>1478</v>
       </c>
       <c r="B556" t="s">
-        <v>1491</v>
+        <v>1487</v>
       </c>
       <c r="C556" s="1" t="s">
-        <v>1491</v>
+        <v>1487</v>
       </c>
       <c r="D556" s="1" t="s">
-        <v>1492</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="557" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14259,13 +14271,13 @@
         <v>1478</v>
       </c>
       <c r="B557" t="s">
-        <v>1493</v>
+        <v>1489</v>
       </c>
       <c r="C557" s="1" t="s">
-        <v>1493</v>
+        <v>1489</v>
       </c>
       <c r="D557" s="1" t="s">
-        <v>1494</v>
+        <v>1490</v>
       </c>
     </row>
     <row r="558" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14273,13 +14285,13 @@
         <v>1478</v>
       </c>
       <c r="B558" t="s">
-        <v>1495</v>
+        <v>1491</v>
       </c>
       <c r="C558" s="1" t="s">
-        <v>1495</v>
+        <v>1491</v>
       </c>
       <c r="D558" s="1" t="s">
-        <v>1496</v>
+        <v>1492</v>
       </c>
     </row>
     <row r="559" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14287,13 +14299,13 @@
         <v>1478</v>
       </c>
       <c r="B559" t="s">
-        <v>1497</v>
+        <v>1493</v>
       </c>
       <c r="C559" s="1" t="s">
-        <v>1497</v>
+        <v>1493</v>
       </c>
       <c r="D559" s="1" t="s">
-        <v>1498</v>
+        <v>1494</v>
       </c>
     </row>
     <row r="560" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14301,13 +14313,13 @@
         <v>1478</v>
       </c>
       <c r="B560" t="s">
-        <v>1499</v>
+        <v>1495</v>
       </c>
       <c r="C560" s="1" t="s">
-        <v>1499</v>
+        <v>1495</v>
       </c>
       <c r="D560" s="1" t="s">
-        <v>1500</v>
+        <v>1496</v>
       </c>
     </row>
     <row r="561" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14315,41 +14327,41 @@
         <v>1478</v>
       </c>
       <c r="B561" t="s">
-        <v>1501</v>
+        <v>1497</v>
       </c>
       <c r="C561" s="1" t="s">
-        <v>1501</v>
+        <v>1497</v>
       </c>
       <c r="D561" s="1" t="s">
-        <v>1502</v>
+        <v>1498</v>
       </c>
     </row>
     <row r="562" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A562" t="s">
-        <v>1503</v>
+        <v>1478</v>
       </c>
       <c r="B562" t="s">
-        <v>1504</v>
+        <v>1499</v>
       </c>
       <c r="C562" s="1" t="s">
-        <v>1504</v>
+        <v>1499</v>
       </c>
       <c r="D562" s="1" t="s">
-        <v>1505</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="563" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A563" t="s">
-        <v>1503</v>
+        <v>1478</v>
       </c>
       <c r="B563" t="s">
-        <v>1506</v>
+        <v>1501</v>
       </c>
       <c r="C563" s="1" t="s">
-        <v>1506</v>
+        <v>1501</v>
       </c>
       <c r="D563" s="1" t="s">
-        <v>1507</v>
+        <v>1502</v>
       </c>
     </row>
     <row r="564" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14357,13 +14369,13 @@
         <v>1503</v>
       </c>
       <c r="B564" t="s">
-        <v>1508</v>
+        <v>1504</v>
       </c>
       <c r="C564" s="1" t="s">
-        <v>1508</v>
+        <v>1504</v>
       </c>
       <c r="D564" s="1" t="s">
-        <v>1509</v>
+        <v>1505</v>
       </c>
     </row>
     <row r="565" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14371,13 +14383,13 @@
         <v>1503</v>
       </c>
       <c r="B565" t="s">
-        <v>1510</v>
+        <v>1506</v>
       </c>
       <c r="C565" s="1" t="s">
-        <v>1510</v>
+        <v>1506</v>
       </c>
       <c r="D565" s="1" t="s">
-        <v>1511</v>
+        <v>1507</v>
       </c>
     </row>
     <row r="566" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14385,13 +14397,13 @@
         <v>1503</v>
       </c>
       <c r="B566" t="s">
-        <v>1512</v>
+        <v>1508</v>
       </c>
       <c r="C566" s="1" t="s">
-        <v>1512</v>
+        <v>1508</v>
       </c>
       <c r="D566" s="1" t="s">
-        <v>1513</v>
+        <v>1509</v>
       </c>
     </row>
     <row r="567" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14399,13 +14411,13 @@
         <v>1503</v>
       </c>
       <c r="B567" t="s">
-        <v>1514</v>
+        <v>1510</v>
       </c>
       <c r="C567" s="1" t="s">
-        <v>1514</v>
+        <v>1510</v>
       </c>
       <c r="D567" s="1" t="s">
-        <v>1515</v>
+        <v>1511</v>
       </c>
     </row>
     <row r="568" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14413,13 +14425,13 @@
         <v>1503</v>
       </c>
       <c r="B568" t="s">
-        <v>1516</v>
+        <v>1512</v>
       </c>
       <c r="C568" s="1" t="s">
-        <v>1516</v>
+        <v>1512</v>
       </c>
       <c r="D568" s="1" t="s">
-        <v>1517</v>
+        <v>1513</v>
       </c>
     </row>
     <row r="569" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14427,13 +14439,13 @@
         <v>1503</v>
       </c>
       <c r="B569" t="s">
-        <v>1518</v>
+        <v>1514</v>
       </c>
       <c r="C569" s="1" t="s">
-        <v>1518</v>
+        <v>1514</v>
       </c>
       <c r="D569" s="1" t="s">
-        <v>1519</v>
+        <v>1515</v>
       </c>
     </row>
     <row r="570" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14441,13 +14453,13 @@
         <v>1503</v>
       </c>
       <c r="B570" t="s">
-        <v>1520</v>
+        <v>1516</v>
       </c>
       <c r="C570" s="1" t="s">
-        <v>1520</v>
+        <v>1516</v>
       </c>
       <c r="D570" s="1" t="s">
-        <v>1521</v>
+        <v>1517</v>
       </c>
     </row>
     <row r="571" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14455,13 +14467,13 @@
         <v>1503</v>
       </c>
       <c r="B571" t="s">
-        <v>1522</v>
+        <v>1518</v>
       </c>
       <c r="C571" s="1" t="s">
-        <v>1522</v>
+        <v>1518</v>
       </c>
       <c r="D571" s="1" t="s">
-        <v>1523</v>
+        <v>1519</v>
       </c>
     </row>
     <row r="572" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14469,13 +14481,13 @@
         <v>1503</v>
       </c>
       <c r="B572" t="s">
-        <v>1524</v>
+        <v>1520</v>
       </c>
       <c r="C572" s="1" t="s">
-        <v>1524</v>
+        <v>1520</v>
       </c>
       <c r="D572" s="1" t="s">
-        <v>1525</v>
+        <v>1521</v>
       </c>
     </row>
     <row r="573" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14483,13 +14495,13 @@
         <v>1503</v>
       </c>
       <c r="B573" t="s">
-        <v>1526</v>
+        <v>1522</v>
       </c>
       <c r="C573" s="1" t="s">
-        <v>1526</v>
+        <v>1522</v>
       </c>
       <c r="D573" s="1" t="s">
-        <v>1527</v>
+        <v>1523</v>
       </c>
     </row>
     <row r="574" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14497,13 +14509,13 @@
         <v>1503</v>
       </c>
       <c r="B574" t="s">
-        <v>1528</v>
+        <v>1524</v>
       </c>
       <c r="C574" s="1" t="s">
-        <v>1528</v>
+        <v>1524</v>
       </c>
       <c r="D574" s="1" t="s">
-        <v>1529</v>
+        <v>1525</v>
       </c>
     </row>
     <row r="575" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14511,69 +14523,69 @@
         <v>1503</v>
       </c>
       <c r="B575" t="s">
-        <v>1530</v>
+        <v>1526</v>
       </c>
       <c r="C575" s="1" t="s">
-        <v>1530</v>
+        <v>1526</v>
       </c>
       <c r="D575" s="1" t="s">
-        <v>1531</v>
+        <v>1527</v>
       </c>
     </row>
     <row r="576" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A576" t="s">
-        <v>1532</v>
+        <v>1503</v>
       </c>
       <c r="B576" t="s">
-        <v>1533</v>
+        <v>1528</v>
       </c>
       <c r="C576" s="1" t="s">
-        <v>1533</v>
+        <v>1528</v>
       </c>
       <c r="D576" s="1" t="s">
-        <v>1534</v>
+        <v>1529</v>
       </c>
     </row>
     <row r="577" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A577" t="s">
-        <v>1532</v>
+        <v>1503</v>
       </c>
       <c r="B577" t="s">
-        <v>1535</v>
+        <v>1530</v>
       </c>
       <c r="C577" s="1" t="s">
-        <v>1535</v>
+        <v>1530</v>
       </c>
       <c r="D577" s="1" t="s">
-        <v>1536</v>
+        <v>1531</v>
       </c>
     </row>
     <row r="578" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A578" t="s">
-        <v>1537</v>
+        <v>1532</v>
       </c>
       <c r="B578" t="s">
-        <v>1538</v>
+        <v>1533</v>
       </c>
       <c r="C578" s="1" t="s">
-        <v>1538</v>
+        <v>1533</v>
       </c>
       <c r="D578" s="1" t="s">
-        <v>1539</v>
+        <v>1534</v>
       </c>
     </row>
     <row r="579" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A579" t="s">
-        <v>1537</v>
+        <v>1532</v>
       </c>
       <c r="B579" t="s">
-        <v>1540</v>
+        <v>1535</v>
       </c>
       <c r="C579" s="1" t="s">
-        <v>1540</v>
+        <v>1535</v>
       </c>
       <c r="D579" s="1" t="s">
-        <v>1541</v>
+        <v>1536</v>
       </c>
     </row>
     <row r="580" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14581,13 +14593,13 @@
         <v>1537</v>
       </c>
       <c r="B580" t="s">
-        <v>1542</v>
+        <v>1538</v>
       </c>
       <c r="C580" s="1" t="s">
-        <v>1542</v>
+        <v>1538</v>
       </c>
       <c r="D580" s="1" t="s">
-        <v>1543</v>
+        <v>1539</v>
       </c>
     </row>
     <row r="581" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14595,13 +14607,13 @@
         <v>1537</v>
       </c>
       <c r="B581" t="s">
-        <v>1544</v>
+        <v>1540</v>
       </c>
       <c r="C581" s="1" t="s">
-        <v>1544</v>
+        <v>1540</v>
       </c>
       <c r="D581" s="1" t="s">
-        <v>1545</v>
+        <v>1541</v>
       </c>
     </row>
     <row r="582" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14609,13 +14621,13 @@
         <v>1537</v>
       </c>
       <c r="B582" t="s">
-        <v>1367</v>
+        <v>1542</v>
       </c>
       <c r="C582" s="1" t="s">
-        <v>1367</v>
+        <v>1542</v>
       </c>
       <c r="D582" s="1" t="s">
-        <v>1546</v>
+        <v>1543</v>
       </c>
     </row>
     <row r="583" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14623,13 +14635,13 @@
         <v>1537</v>
       </c>
       <c r="B583" t="s">
-        <v>1381</v>
+        <v>1544</v>
       </c>
       <c r="C583" s="1" t="s">
-        <v>1381</v>
+        <v>1544</v>
       </c>
       <c r="D583" s="1" t="s">
-        <v>1547</v>
+        <v>1545</v>
       </c>
     </row>
     <row r="584" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14637,13 +14649,13 @@
         <v>1537</v>
       </c>
       <c r="B584" t="s">
-        <v>1278</v>
+        <v>1367</v>
       </c>
       <c r="C584" s="1" t="s">
-        <v>1278</v>
+        <v>1367</v>
       </c>
       <c r="D584" s="1" t="s">
-        <v>1548</v>
+        <v>1546</v>
       </c>
     </row>
     <row r="585" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14651,13 +14663,13 @@
         <v>1537</v>
       </c>
       <c r="B585" t="s">
-        <v>1549</v>
+        <v>1381</v>
       </c>
       <c r="C585" s="1" t="s">
-        <v>1549</v>
+        <v>1381</v>
       </c>
       <c r="D585" s="1" t="s">
-        <v>1550</v>
+        <v>1547</v>
       </c>
     </row>
     <row r="586" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14665,13 +14677,13 @@
         <v>1537</v>
       </c>
       <c r="B586" t="s">
-        <v>1551</v>
+        <v>1278</v>
       </c>
       <c r="C586" s="1" t="s">
-        <v>1551</v>
+        <v>1278</v>
       </c>
       <c r="D586" s="1" t="s">
-        <v>1552</v>
+        <v>1548</v>
       </c>
     </row>
     <row r="587" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14679,13 +14691,13 @@
         <v>1537</v>
       </c>
       <c r="B587" t="s">
-        <v>1553</v>
+        <v>1549</v>
       </c>
       <c r="C587" s="1" t="s">
-        <v>1553</v>
+        <v>1549</v>
       </c>
       <c r="D587" s="1" t="s">
-        <v>1554</v>
+        <v>1550</v>
       </c>
     </row>
     <row r="588" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14693,13 +14705,13 @@
         <v>1537</v>
       </c>
       <c r="B588" t="s">
-        <v>1555</v>
+        <v>1551</v>
       </c>
       <c r="C588" s="1" t="s">
-        <v>1555</v>
+        <v>1551</v>
       </c>
       <c r="D588" s="1" t="s">
-        <v>1556</v>
+        <v>1552</v>
       </c>
     </row>
     <row r="589" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14707,41 +14719,41 @@
         <v>1537</v>
       </c>
       <c r="B589" t="s">
-        <v>1557</v>
+        <v>1553</v>
       </c>
       <c r="C589" s="1" t="s">
-        <v>1557</v>
+        <v>1553</v>
       </c>
       <c r="D589" s="1" t="s">
-        <v>1558</v>
+        <v>1554</v>
       </c>
     </row>
     <row r="590" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A590" t="s">
-        <v>1559</v>
+        <v>1537</v>
       </c>
       <c r="B590" t="s">
-        <v>1560</v>
+        <v>1555</v>
       </c>
       <c r="C590" s="1" t="s">
-        <v>1560</v>
+        <v>1555</v>
       </c>
       <c r="D590" s="1" t="s">
-        <v>1561</v>
+        <v>1556</v>
       </c>
     </row>
     <row r="591" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A591" t="s">
-        <v>1559</v>
+        <v>1537</v>
       </c>
       <c r="B591" t="s">
-        <v>1562</v>
+        <v>1557</v>
       </c>
       <c r="C591" s="1" t="s">
-        <v>1562</v>
+        <v>1557</v>
       </c>
       <c r="D591" s="1" t="s">
-        <v>1563</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="592" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14749,69 +14761,69 @@
         <v>1559</v>
       </c>
       <c r="B592" t="s">
-        <v>1564</v>
+        <v>1560</v>
       </c>
       <c r="C592" s="1" t="s">
-        <v>1564</v>
+        <v>1560</v>
       </c>
       <c r="D592" s="1" t="s">
-        <v>1565</v>
+        <v>1561</v>
       </c>
     </row>
     <row r="593" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A593" t="s">
-        <v>1566</v>
+        <v>1559</v>
       </c>
       <c r="B593" t="s">
-        <v>1567</v>
+        <v>1562</v>
       </c>
       <c r="C593" s="1" t="s">
-        <v>1567</v>
+        <v>1562</v>
       </c>
       <c r="D593" s="1" t="s">
-        <v>1568</v>
-      </c>
-    </row>
-    <row r="594" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>1563</v>
+      </c>
+    </row>
+    <row r="594" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A594" t="s">
-        <v>1566</v>
+        <v>1559</v>
       </c>
       <c r="B594" t="s">
-        <v>1569</v>
+        <v>1564</v>
       </c>
       <c r="C594" s="1" t="s">
-        <v>1569</v>
+        <v>1564</v>
       </c>
       <c r="D594" s="1" t="s">
-        <v>1570</v>
+        <v>1565</v>
       </c>
     </row>
     <row r="595" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A595" t="s">
-        <v>1571</v>
+        <v>1566</v>
       </c>
       <c r="B595" t="s">
-        <v>1572</v>
+        <v>1567</v>
       </c>
       <c r="C595" s="1" t="s">
-        <v>1572</v>
+        <v>1567</v>
       </c>
       <c r="D595" s="1" t="s">
-        <v>1573</v>
-      </c>
-    </row>
-    <row r="596" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>1568</v>
+      </c>
+    </row>
+    <row r="596" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A596" t="s">
-        <v>1571</v>
+        <v>1566</v>
       </c>
       <c r="B596" t="s">
-        <v>1574</v>
+        <v>1569</v>
       </c>
       <c r="C596" s="1" t="s">
-        <v>1574</v>
+        <v>1569</v>
       </c>
       <c r="D596" s="1" t="s">
-        <v>1575</v>
+        <v>1570</v>
       </c>
     </row>
     <row r="597" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14819,167 +14831,167 @@
         <v>1571</v>
       </c>
       <c r="B597" t="s">
-        <v>1576</v>
+        <v>1572</v>
       </c>
       <c r="C597" s="1" t="s">
-        <v>1576</v>
+        <v>1572</v>
       </c>
       <c r="D597" s="1" t="s">
-        <v>1577</v>
-      </c>
-    </row>
-    <row r="598" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>1573</v>
+      </c>
+    </row>
+    <row r="598" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A598" t="s">
         <v>1571</v>
       </c>
       <c r="B598" t="s">
-        <v>1578</v>
+        <v>1574</v>
       </c>
       <c r="C598" s="1" t="s">
-        <v>1578</v>
+        <v>1574</v>
       </c>
       <c r="D598" s="1" t="s">
-        <v>1579</v>
+        <v>1575</v>
       </c>
     </row>
     <row r="599" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A599" t="s">
-        <v>1580</v>
+        <v>1571</v>
       </c>
       <c r="B599" t="s">
-        <v>1581</v>
+        <v>1576</v>
       </c>
       <c r="C599" s="1" t="s">
-        <v>1581</v>
+        <v>1576</v>
       </c>
       <c r="D599" s="1" t="s">
-        <v>1582</v>
-      </c>
-    </row>
-    <row r="600" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>1577</v>
+      </c>
+    </row>
+    <row r="600" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A600" t="s">
-        <v>1580</v>
+        <v>1571</v>
       </c>
       <c r="B600" t="s">
-        <v>1583</v>
+        <v>1578</v>
       </c>
       <c r="C600" s="1" t="s">
-        <v>1583</v>
+        <v>1578</v>
       </c>
       <c r="D600" s="1" t="s">
-        <v>1584</v>
+        <v>1579</v>
       </c>
     </row>
     <row r="601" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A601" t="s">
-        <v>1585</v>
+        <v>1580</v>
       </c>
       <c r="B601" t="s">
-        <v>1586</v>
+        <v>1581</v>
       </c>
       <c r="C601" s="1" t="s">
-        <v>1586</v>
+        <v>1581</v>
       </c>
       <c r="D601" s="1" t="s">
-        <v>1587</v>
-      </c>
-    </row>
-    <row r="602" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>1582</v>
+      </c>
+    </row>
+    <row r="602" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A602" t="s">
-        <v>1585</v>
+        <v>1580</v>
       </c>
       <c r="B602" t="s">
-        <v>1588</v>
+        <v>1583</v>
       </c>
       <c r="C602" s="1" t="s">
-        <v>1588</v>
+        <v>1583</v>
       </c>
       <c r="D602" s="1" t="s">
-        <v>1589</v>
+        <v>1584</v>
       </c>
     </row>
     <row r="603" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A603" t="s">
-        <v>1590</v>
+        <v>1585</v>
       </c>
       <c r="B603" t="s">
-        <v>1591</v>
+        <v>1586</v>
       </c>
       <c r="C603" s="1" t="s">
-        <v>1591</v>
+        <v>1586</v>
       </c>
       <c r="D603" s="1" t="s">
-        <v>1592</v>
+        <v>1587</v>
       </c>
     </row>
     <row r="604" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A604" t="s">
-        <v>1590</v>
+        <v>1585</v>
       </c>
       <c r="B604" t="s">
-        <v>1593</v>
+        <v>1588</v>
       </c>
       <c r="C604" s="1" t="s">
-        <v>1593</v>
+        <v>1588</v>
       </c>
       <c r="D604" s="1" t="s">
-        <v>1594</v>
+        <v>1589</v>
       </c>
     </row>
     <row r="605" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A605" t="s">
-        <v>1595</v>
+        <v>1590</v>
       </c>
       <c r="B605" t="s">
-        <v>1596</v>
+        <v>1591</v>
       </c>
       <c r="C605" s="1" t="s">
-        <v>1596</v>
+        <v>1591</v>
       </c>
       <c r="D605" s="1" t="s">
-        <v>1597</v>
-      </c>
-    </row>
-    <row r="606" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>1592</v>
+      </c>
+    </row>
+    <row r="606" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A606" t="s">
-        <v>1595</v>
+        <v>1590</v>
       </c>
       <c r="B606" t="s">
-        <v>1598</v>
+        <v>1593</v>
       </c>
       <c r="C606" s="1" t="s">
-        <v>1598</v>
+        <v>1593</v>
       </c>
       <c r="D606" s="1" t="s">
-        <v>1599</v>
+        <v>1594</v>
       </c>
     </row>
     <row r="607" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A607" t="s">
-        <v>1600</v>
+        <v>1595</v>
       </c>
       <c r="B607" t="s">
-        <v>1601</v>
+        <v>1596</v>
       </c>
       <c r="C607" s="1" t="s">
-        <v>1601</v>
+        <v>1596</v>
       </c>
       <c r="D607" s="1" t="s">
-        <v>1602</v>
-      </c>
-    </row>
-    <row r="608" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>1597</v>
+      </c>
+    </row>
+    <row r="608" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A608" t="s">
-        <v>1600</v>
+        <v>1595</v>
       </c>
       <c r="B608" t="s">
-        <v>1603</v>
+        <v>1598</v>
       </c>
       <c r="C608" s="1" t="s">
-        <v>1603</v>
+        <v>1598</v>
       </c>
       <c r="D608" s="1" t="s">
-        <v>1604</v>
+        <v>1599</v>
       </c>
     </row>
     <row r="609" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14987,41 +14999,41 @@
         <v>1600</v>
       </c>
       <c r="B609" t="s">
-        <v>1605</v>
+        <v>1601</v>
       </c>
       <c r="C609" s="1" t="s">
-        <v>1605</v>
+        <v>1601</v>
       </c>
       <c r="D609" s="1" t="s">
-        <v>1606</v>
-      </c>
-    </row>
-    <row r="610" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>1602</v>
+      </c>
+    </row>
+    <row r="610" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A610" t="s">
         <v>1600</v>
       </c>
       <c r="B610" t="s">
-        <v>1607</v>
+        <v>1603</v>
       </c>
       <c r="C610" s="1" t="s">
-        <v>1607</v>
+        <v>1603</v>
       </c>
       <c r="D610" s="1" t="s">
-        <v>1608</v>
-      </c>
-    </row>
-    <row r="611" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>1604</v>
+      </c>
+    </row>
+    <row r="611" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A611" t="s">
         <v>1600</v>
       </c>
       <c r="B611" t="s">
-        <v>1609</v>
+        <v>1605</v>
       </c>
       <c r="C611" s="1" t="s">
-        <v>1609</v>
+        <v>1605</v>
       </c>
       <c r="D611" s="1" t="s">
-        <v>1610</v>
+        <v>1606</v>
       </c>
     </row>
     <row r="612" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -15029,41 +15041,41 @@
         <v>1600</v>
       </c>
       <c r="B612" t="s">
-        <v>1611</v>
+        <v>1607</v>
       </c>
       <c r="C612" s="1" t="s">
-        <v>1611</v>
+        <v>1607</v>
       </c>
       <c r="D612" s="1" t="s">
-        <v>1612</v>
-      </c>
-    </row>
-    <row r="613" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>1608</v>
+      </c>
+    </row>
+    <row r="613" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A613" t="s">
         <v>1600</v>
       </c>
       <c r="B613" t="s">
-        <v>1613</v>
+        <v>1609</v>
       </c>
       <c r="C613" s="1" t="s">
-        <v>1613</v>
+        <v>1609</v>
       </c>
       <c r="D613" s="1" t="s">
-        <v>1614</v>
-      </c>
-    </row>
-    <row r="614" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>1610</v>
+      </c>
+    </row>
+    <row r="614" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A614" t="s">
         <v>1600</v>
       </c>
       <c r="B614" t="s">
-        <v>1615</v>
+        <v>1611</v>
       </c>
       <c r="C614" s="1" t="s">
-        <v>1615</v>
+        <v>1611</v>
       </c>
       <c r="D614" s="1" t="s">
-        <v>1616</v>
+        <v>1612</v>
       </c>
     </row>
     <row r="615" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -15071,27 +15083,27 @@
         <v>1600</v>
       </c>
       <c r="B615" t="s">
-        <v>1617</v>
+        <v>1613</v>
       </c>
       <c r="C615" s="1" t="s">
-        <v>1617</v>
+        <v>1613</v>
       </c>
       <c r="D615" s="1" t="s">
-        <v>1618</v>
-      </c>
-    </row>
-    <row r="616" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>1614</v>
+      </c>
+    </row>
+    <row r="616" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A616" t="s">
         <v>1600</v>
       </c>
       <c r="B616" t="s">
-        <v>1619</v>
+        <v>1615</v>
       </c>
       <c r="C616" s="1" t="s">
-        <v>1619</v>
+        <v>1615</v>
       </c>
       <c r="D616" s="1" t="s">
-        <v>1620</v>
+        <v>1616</v>
       </c>
     </row>
     <row r="617" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -15099,13 +15111,13 @@
         <v>1600</v>
       </c>
       <c r="B617" t="s">
-        <v>1621</v>
+        <v>1617</v>
       </c>
       <c r="C617" s="1" t="s">
-        <v>1621</v>
+        <v>1617</v>
       </c>
       <c r="D617" s="1" t="s">
-        <v>1622</v>
+        <v>1618</v>
       </c>
     </row>
     <row r="618" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -15113,13 +15125,13 @@
         <v>1600</v>
       </c>
       <c r="B618" t="s">
-        <v>1623</v>
+        <v>1619</v>
       </c>
       <c r="C618" s="1" t="s">
-        <v>1623</v>
+        <v>1619</v>
       </c>
       <c r="D618" s="1" t="s">
-        <v>1624</v>
+        <v>1620</v>
       </c>
     </row>
     <row r="619" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -15127,13 +15139,13 @@
         <v>1600</v>
       </c>
       <c r="B619" t="s">
-        <v>1625</v>
+        <v>1621</v>
       </c>
       <c r="C619" s="1" t="s">
-        <v>1625</v>
+        <v>1621</v>
       </c>
       <c r="D619" s="1" t="s">
-        <v>1626</v>
+        <v>1622</v>
       </c>
     </row>
     <row r="620" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -15141,13 +15153,13 @@
         <v>1600</v>
       </c>
       <c r="B620" t="s">
-        <v>1627</v>
+        <v>1623</v>
       </c>
       <c r="C620" s="1" t="s">
-        <v>1627</v>
+        <v>1623</v>
       </c>
       <c r="D620" s="1" t="s">
-        <v>1628</v>
+        <v>1624</v>
       </c>
     </row>
     <row r="621" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -15155,13 +15167,13 @@
         <v>1600</v>
       </c>
       <c r="B621" t="s">
-        <v>1629</v>
+        <v>1625</v>
       </c>
       <c r="C621" s="1" t="s">
-        <v>1629</v>
+        <v>1625</v>
       </c>
       <c r="D621" s="1" t="s">
-        <v>1630</v>
+        <v>1626</v>
       </c>
     </row>
     <row r="622" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -15169,69 +15181,69 @@
         <v>1600</v>
       </c>
       <c r="B622" t="s">
-        <v>1631</v>
+        <v>1627</v>
       </c>
       <c r="C622" s="1" t="s">
-        <v>1631</v>
+        <v>1627</v>
       </c>
       <c r="D622" s="1" t="s">
-        <v>1632</v>
-      </c>
-    </row>
-    <row r="623" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>1628</v>
+      </c>
+    </row>
+    <row r="623" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A623" t="s">
         <v>1600</v>
       </c>
       <c r="B623" t="s">
-        <v>1633</v>
+        <v>1629</v>
       </c>
       <c r="C623" s="1" t="s">
-        <v>1633</v>
+        <v>1629</v>
       </c>
       <c r="D623" s="1" t="s">
-        <v>1634</v>
-      </c>
-    </row>
-    <row r="624" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+        <v>1630</v>
+      </c>
+    </row>
+    <row r="624" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A624" t="s">
         <v>1600</v>
       </c>
       <c r="B624" t="s">
-        <v>1635</v>
+        <v>1631</v>
       </c>
       <c r="C624" s="1" t="s">
-        <v>1635</v>
+        <v>1631</v>
       </c>
       <c r="D624" s="1" t="s">
-        <v>1636</v>
-      </c>
-    </row>
-    <row r="625" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+        <v>1632</v>
+      </c>
+    </row>
+    <row r="625" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A625" t="s">
         <v>1600</v>
       </c>
       <c r="B625" t="s">
-        <v>1637</v>
+        <v>1633</v>
       </c>
       <c r="C625" s="1" t="s">
-        <v>1637</v>
+        <v>1633</v>
       </c>
       <c r="D625" s="1" t="s">
-        <v>1638</v>
-      </c>
-    </row>
-    <row r="626" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+        <v>1634</v>
+      </c>
+    </row>
+    <row r="626" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A626" t="s">
         <v>1600</v>
       </c>
       <c r="B626" t="s">
-        <v>1639</v>
+        <v>1635</v>
       </c>
       <c r="C626" s="1" t="s">
-        <v>1639</v>
+        <v>1635</v>
       </c>
       <c r="D626" s="1" t="s">
-        <v>1640</v>
+        <v>1636</v>
       </c>
     </row>
     <row r="627" spans="1:4" ht="85" x14ac:dyDescent="0.2">
@@ -15239,41 +15251,41 @@
         <v>1600</v>
       </c>
       <c r="B627" t="s">
+        <v>1637</v>
+      </c>
+      <c r="C627" s="1" t="s">
+        <v>1637</v>
+      </c>
+      <c r="D627" s="1" t="s">
+        <v>1638</v>
+      </c>
+    </row>
+    <row r="628" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A628" t="s">
+        <v>1600</v>
+      </c>
+      <c r="B628" t="s">
+        <v>1639</v>
+      </c>
+      <c r="C628" s="1" t="s">
+        <v>1639</v>
+      </c>
+      <c r="D628" s="1" t="s">
+        <v>1640</v>
+      </c>
+    </row>
+    <row r="629" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A629" t="s">
+        <v>1600</v>
+      </c>
+      <c r="B629" t="s">
         <v>1641</v>
       </c>
-      <c r="C627" s="1" t="s">
+      <c r="C629" s="1" t="s">
         <v>1641</v>
       </c>
-      <c r="D627" s="1" t="s">
+      <c r="D629" s="1" t="s">
         <v>1642</v>
-      </c>
-    </row>
-    <row r="628" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A628" t="s">
-        <v>1643</v>
-      </c>
-      <c r="B628" t="s">
-        <v>1644</v>
-      </c>
-      <c r="C628" s="1" t="s">
-        <v>1644</v>
-      </c>
-      <c r="D628" s="1" t="s">
-        <v>1645</v>
-      </c>
-    </row>
-    <row r="629" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A629" t="s">
-        <v>1643</v>
-      </c>
-      <c r="B629" t="s">
-        <v>1646</v>
-      </c>
-      <c r="C629" s="1" t="s">
-        <v>1646</v>
-      </c>
-      <c r="D629" s="1" t="s">
-        <v>1647</v>
       </c>
     </row>
     <row r="630" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -15281,27 +15293,27 @@
         <v>1643</v>
       </c>
       <c r="B630" t="s">
-        <v>1648</v>
+        <v>1644</v>
       </c>
       <c r="C630" s="1" t="s">
-        <v>1648</v>
+        <v>1644</v>
       </c>
       <c r="D630" s="1" t="s">
-        <v>1649</v>
-      </c>
-    </row>
-    <row r="631" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>1645</v>
+      </c>
+    </row>
+    <row r="631" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A631" t="s">
         <v>1643</v>
       </c>
       <c r="B631" t="s">
-        <v>1650</v>
+        <v>1646</v>
       </c>
       <c r="C631" s="1" t="s">
-        <v>1650</v>
+        <v>1646</v>
       </c>
       <c r="D631" s="1" t="s">
-        <v>1651</v>
+        <v>1647</v>
       </c>
     </row>
     <row r="632" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -15309,69 +15321,69 @@
         <v>1643</v>
       </c>
       <c r="B632" t="s">
-        <v>185</v>
+        <v>1648</v>
       </c>
       <c r="C632" s="1" t="s">
-        <v>185</v>
+        <v>1648</v>
       </c>
       <c r="D632" s="1" t="s">
-        <v>1652</v>
-      </c>
-    </row>
-    <row r="633" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>1649</v>
+      </c>
+    </row>
+    <row r="633" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A633" t="s">
-        <v>1653</v>
+        <v>1643</v>
       </c>
       <c r="B633" t="s">
-        <v>1654</v>
+        <v>1650</v>
       </c>
       <c r="C633" s="1" t="s">
-        <v>1654</v>
+        <v>1650</v>
       </c>
       <c r="D633" s="1" t="s">
-        <v>1655</v>
+        <v>1651</v>
       </c>
     </row>
     <row r="634" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A634" t="s">
-        <v>1653</v>
+        <v>1643</v>
       </c>
       <c r="B634" t="s">
-        <v>1656</v>
+        <v>185</v>
       </c>
       <c r="C634" s="1" t="s">
-        <v>1656</v>
+        <v>185</v>
       </c>
       <c r="D634" s="1" t="s">
-        <v>1657</v>
+        <v>1652</v>
       </c>
     </row>
     <row r="635" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A635" t="s">
-        <v>1658</v>
+        <v>1653</v>
       </c>
       <c r="B635" t="s">
-        <v>1659</v>
+        <v>1654</v>
       </c>
       <c r="C635" s="1" t="s">
-        <v>1660</v>
+        <v>1654</v>
       </c>
       <c r="D635" s="1" t="s">
-        <v>1661</v>
+        <v>1655</v>
       </c>
     </row>
     <row r="636" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A636" t="s">
-        <v>1658</v>
+        <v>1653</v>
       </c>
       <c r="B636" t="s">
-        <v>1654</v>
+        <v>1656</v>
       </c>
       <c r="C636" s="1" t="s">
-        <v>1654</v>
+        <v>1656</v>
       </c>
       <c r="D636" s="1" t="s">
-        <v>1662</v>
+        <v>1657</v>
       </c>
     </row>
     <row r="637" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -15379,13 +15391,13 @@
         <v>1658</v>
       </c>
       <c r="B637" t="s">
-        <v>1663</v>
+        <v>1659</v>
       </c>
       <c r="C637" s="1" t="s">
-        <v>1663</v>
+        <v>1660</v>
       </c>
       <c r="D637" s="1" t="s">
-        <v>1664</v>
+        <v>1661</v>
       </c>
     </row>
     <row r="638" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -15393,83 +15405,83 @@
         <v>1658</v>
       </c>
       <c r="B638" t="s">
-        <v>1665</v>
+        <v>1654</v>
       </c>
       <c r="C638" s="1" t="s">
-        <v>1665</v>
+        <v>1654</v>
       </c>
       <c r="D638" s="1" t="s">
-        <v>1666</v>
-      </c>
-    </row>
-    <row r="639" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>1662</v>
+      </c>
+    </row>
+    <row r="639" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A639" t="s">
         <v>1658</v>
       </c>
       <c r="B639" t="s">
-        <v>1667</v>
+        <v>1663</v>
       </c>
       <c r="C639" s="1" t="s">
-        <v>1667</v>
+        <v>1663</v>
       </c>
       <c r="D639" s="1" t="s">
-        <v>1668</v>
+        <v>1664</v>
       </c>
     </row>
     <row r="640" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A640" t="s">
-        <v>1669</v>
+        <v>1658</v>
       </c>
       <c r="B640" t="s">
-        <v>1670</v>
+        <v>1665</v>
       </c>
       <c r="C640" s="1" t="s">
-        <v>1670</v>
+        <v>1665</v>
       </c>
       <c r="D640" s="1" t="s">
-        <v>1671</v>
+        <v>1666</v>
       </c>
     </row>
     <row r="641" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A641" t="s">
-        <v>1669</v>
+        <v>1658</v>
       </c>
       <c r="B641" t="s">
-        <v>1672</v>
+        <v>1667</v>
       </c>
       <c r="C641" s="1" t="s">
-        <v>1672</v>
+        <v>1667</v>
       </c>
       <c r="D641" s="1" t="s">
-        <v>1671</v>
+        <v>1668</v>
       </c>
     </row>
     <row r="642" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A642" t="s">
-        <v>1673</v>
+        <v>1669</v>
       </c>
       <c r="B642" t="s">
-        <v>1674</v>
+        <v>1670</v>
       </c>
       <c r="C642" s="1" t="s">
-        <v>1674</v>
+        <v>1670</v>
       </c>
       <c r="D642" s="1" t="s">
-        <v>1675</v>
+        <v>1671</v>
       </c>
     </row>
     <row r="643" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A643" t="s">
-        <v>1673</v>
+        <v>1669</v>
       </c>
       <c r="B643" t="s">
-        <v>1676</v>
+        <v>1672</v>
       </c>
       <c r="C643" s="1" t="s">
-        <v>1676</v>
+        <v>1672</v>
       </c>
       <c r="D643" s="1" t="s">
-        <v>1677</v>
+        <v>1671</v>
       </c>
     </row>
     <row r="644" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -15477,13 +15489,13 @@
         <v>1673</v>
       </c>
       <c r="B644" t="s">
-        <v>1678</v>
+        <v>1674</v>
       </c>
       <c r="C644" s="1" t="s">
-        <v>1678</v>
+        <v>1674</v>
       </c>
       <c r="D644" s="1" t="s">
-        <v>1679</v>
+        <v>1675</v>
       </c>
     </row>
     <row r="645" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -15491,13 +15503,13 @@
         <v>1673</v>
       </c>
       <c r="B645" t="s">
-        <v>1680</v>
+        <v>1676</v>
       </c>
       <c r="C645" s="1" t="s">
-        <v>1680</v>
+        <v>1676</v>
       </c>
       <c r="D645" s="1" t="s">
-        <v>1681</v>
+        <v>1677</v>
       </c>
     </row>
     <row r="646" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -15505,41 +15517,41 @@
         <v>1673</v>
       </c>
       <c r="B646" t="s">
-        <v>1682</v>
+        <v>1678</v>
       </c>
       <c r="C646" s="1" t="s">
-        <v>1682</v>
+        <v>1678</v>
       </c>
       <c r="D646" s="1" t="s">
-        <v>1683</v>
+        <v>1679</v>
       </c>
     </row>
     <row r="647" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A647" t="s">
-        <v>1684</v>
+        <v>1673</v>
       </c>
       <c r="B647" t="s">
-        <v>1685</v>
+        <v>1680</v>
       </c>
       <c r="C647" s="1" t="s">
-        <v>1685</v>
+        <v>1680</v>
       </c>
       <c r="D647" s="1" t="s">
-        <v>1686</v>
+        <v>1681</v>
       </c>
     </row>
     <row r="648" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A648" t="s">
-        <v>1684</v>
+        <v>1673</v>
       </c>
       <c r="B648" t="s">
-        <v>1687</v>
+        <v>1682</v>
       </c>
       <c r="C648" s="1" t="s">
-        <v>1687</v>
+        <v>1682</v>
       </c>
       <c r="D648" s="1" t="s">
-        <v>1688</v>
+        <v>1683</v>
       </c>
     </row>
     <row r="649" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -15547,13 +15559,13 @@
         <v>1684</v>
       </c>
       <c r="B649" t="s">
-        <v>1689</v>
+        <v>1685</v>
       </c>
       <c r="C649" s="1" t="s">
-        <v>1689</v>
+        <v>1685</v>
       </c>
       <c r="D649" s="1" t="s">
-        <v>1690</v>
+        <v>1686</v>
       </c>
     </row>
     <row r="650" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -15561,153 +15573,153 @@
         <v>1684</v>
       </c>
       <c r="B650" t="s">
-        <v>1691</v>
+        <v>1687</v>
       </c>
       <c r="C650" s="1" t="s">
-        <v>1691</v>
+        <v>1687</v>
       </c>
       <c r="D650" s="1" t="s">
-        <v>1692</v>
+        <v>1688</v>
       </c>
     </row>
     <row r="651" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A651" t="s">
-        <v>1693</v>
+        <v>1684</v>
       </c>
       <c r="B651" t="s">
-        <v>1694</v>
+        <v>1689</v>
       </c>
       <c r="C651" s="1" t="s">
-        <v>1694</v>
+        <v>1689</v>
       </c>
       <c r="D651" s="1" t="s">
-        <v>1695</v>
+        <v>1690</v>
       </c>
     </row>
     <row r="652" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A652" t="s">
-        <v>1693</v>
+        <v>1684</v>
       </c>
       <c r="B652" t="s">
-        <v>1696</v>
+        <v>1691</v>
       </c>
       <c r="C652" s="1" t="s">
-        <v>1696</v>
+        <v>1691</v>
       </c>
       <c r="D652" s="1" t="s">
-        <v>1695</v>
+        <v>1692</v>
       </c>
     </row>
     <row r="653" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A653" t="s">
-        <v>1673</v>
+        <v>1693</v>
       </c>
       <c r="B653" t="s">
-        <v>1697</v>
+        <v>1694</v>
       </c>
       <c r="C653" s="1" t="s">
-        <v>1697</v>
+        <v>1694</v>
       </c>
       <c r="D653" s="1" t="s">
-        <v>1698</v>
+        <v>1695</v>
       </c>
     </row>
     <row r="654" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A654" t="s">
-        <v>1699</v>
+        <v>1693</v>
       </c>
       <c r="B654" t="s">
-        <v>1700</v>
+        <v>1696</v>
       </c>
       <c r="C654" s="1" t="s">
-        <v>1700</v>
+        <v>1696</v>
       </c>
       <c r="D654" s="1" t="s">
-        <v>1698</v>
-      </c>
-    </row>
-    <row r="655" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>1695</v>
+      </c>
+    </row>
+    <row r="655" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A655" t="s">
-        <v>1699</v>
+        <v>1673</v>
       </c>
       <c r="B655" t="s">
-        <v>318</v>
+        <v>1697</v>
       </c>
       <c r="C655" s="1" t="s">
-        <v>318</v>
+        <v>1697</v>
       </c>
       <c r="D655" s="1" t="s">
         <v>1698</v>
       </c>
     </row>
-    <row r="656" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="656" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A656" t="s">
         <v>1699</v>
       </c>
       <c r="B656" t="s">
-        <v>1701</v>
+        <v>1700</v>
       </c>
       <c r="C656" s="1" t="s">
-        <v>1701</v>
+        <v>1700</v>
       </c>
       <c r="D656" s="1" t="s">
         <v>1698</v>
       </c>
     </row>
-    <row r="657" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="657" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A657" t="s">
         <v>1699</v>
       </c>
       <c r="B657" t="s">
-        <v>1702</v>
+        <v>318</v>
       </c>
       <c r="C657" s="1" t="s">
-        <v>1702</v>
+        <v>318</v>
       </c>
       <c r="D657" s="1" t="s">
         <v>1698</v>
       </c>
     </row>
-    <row r="658" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="658" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A658" t="s">
         <v>1699</v>
       </c>
       <c r="B658" t="s">
-        <v>1697</v>
+        <v>1701</v>
       </c>
       <c r="C658" s="1" t="s">
-        <v>1697</v>
+        <v>1701</v>
       </c>
       <c r="D658" s="1" t="s">
         <v>1698</v>
       </c>
     </row>
-    <row r="659" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="659" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A659" t="s">
-        <v>1703</v>
+        <v>1699</v>
       </c>
       <c r="B659" t="s">
-        <v>1704</v>
+        <v>1702</v>
       </c>
       <c r="C659" s="1" t="s">
-        <v>1704</v>
+        <v>1702</v>
       </c>
       <c r="D659" s="1" t="s">
-        <v>1705</v>
-      </c>
-    </row>
-    <row r="660" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>1698</v>
+      </c>
+    </row>
+    <row r="660" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A660" t="s">
-        <v>1703</v>
+        <v>1699</v>
       </c>
       <c r="B660" t="s">
-        <v>1706</v>
+        <v>1697</v>
       </c>
       <c r="C660" s="1" t="s">
-        <v>1706</v>
+        <v>1697</v>
       </c>
       <c r="D660" s="1" t="s">
-        <v>1707</v>
+        <v>1698</v>
       </c>
     </row>
     <row r="661" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -15715,69 +15727,69 @@
         <v>1703</v>
       </c>
       <c r="B661" t="s">
-        <v>1708</v>
+        <v>1704</v>
       </c>
       <c r="C661" s="1" t="s">
-        <v>1708</v>
+        <v>1704</v>
       </c>
       <c r="D661" s="1" t="s">
-        <v>1709</v>
+        <v>1705</v>
       </c>
     </row>
     <row r="662" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A662" t="s">
-        <v>1710</v>
+        <v>1703</v>
       </c>
       <c r="B662" t="s">
-        <v>1711</v>
+        <v>1706</v>
       </c>
       <c r="C662" s="1" t="s">
-        <v>1711</v>
+        <v>1706</v>
       </c>
       <c r="D662" s="1" t="s">
-        <v>1712</v>
+        <v>1707</v>
       </c>
     </row>
     <row r="663" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A663" t="s">
-        <v>1710</v>
+        <v>1703</v>
       </c>
       <c r="B663" t="s">
-        <v>1713</v>
+        <v>1708</v>
       </c>
       <c r="C663" s="1" t="s">
-        <v>1713</v>
+        <v>1708</v>
       </c>
       <c r="D663" s="1" t="s">
-        <v>1714</v>
+        <v>1709</v>
       </c>
     </row>
     <row r="664" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A664" t="s">
-        <v>1715</v>
+        <v>1710</v>
       </c>
       <c r="B664" t="s">
-        <v>1716</v>
+        <v>1711</v>
       </c>
       <c r="C664" s="1" t="s">
-        <v>1716</v>
+        <v>1711</v>
       </c>
       <c r="D664" s="1" t="s">
-        <v>1717</v>
+        <v>1712</v>
       </c>
     </row>
     <row r="665" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A665" t="s">
-        <v>1715</v>
+        <v>1710</v>
       </c>
       <c r="B665" t="s">
-        <v>1718</v>
+        <v>1713</v>
       </c>
       <c r="C665" s="1" t="s">
-        <v>1718</v>
+        <v>1713</v>
       </c>
       <c r="D665" s="1" t="s">
-        <v>1719</v>
+        <v>1714</v>
       </c>
     </row>
     <row r="666" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -15785,13 +15797,13 @@
         <v>1715</v>
       </c>
       <c r="B666" t="s">
-        <v>1720</v>
+        <v>1716</v>
       </c>
       <c r="C666" s="1" t="s">
-        <v>1720</v>
+        <v>1716</v>
       </c>
       <c r="D666" s="1" t="s">
-        <v>1721</v>
+        <v>1717</v>
       </c>
     </row>
     <row r="667" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -15799,13 +15811,13 @@
         <v>1715</v>
       </c>
       <c r="B667" t="s">
-        <v>1722</v>
+        <v>1718</v>
       </c>
       <c r="C667" s="1" t="s">
-        <v>1722</v>
+        <v>1718</v>
       </c>
       <c r="D667" s="1" t="s">
-        <v>1723</v>
+        <v>1719</v>
       </c>
     </row>
     <row r="668" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -15813,41 +15825,41 @@
         <v>1715</v>
       </c>
       <c r="B668" t="s">
-        <v>1724</v>
+        <v>1720</v>
       </c>
       <c r="C668" s="1" t="s">
-        <v>1724</v>
+        <v>1720</v>
       </c>
       <c r="D668" s="1" t="s">
-        <v>1725</v>
+        <v>1721</v>
       </c>
     </row>
     <row r="669" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A669" t="s">
-        <v>1726</v>
+        <v>1715</v>
       </c>
       <c r="B669" t="s">
-        <v>129</v>
+        <v>1722</v>
       </c>
       <c r="C669" s="1" t="s">
-        <v>129</v>
+        <v>1722</v>
       </c>
       <c r="D669" s="1" t="s">
-        <v>1727</v>
+        <v>1723</v>
       </c>
     </row>
     <row r="670" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A670" t="s">
-        <v>1726</v>
+        <v>1715</v>
       </c>
       <c r="B670" t="s">
-        <v>1728</v>
+        <v>1724</v>
       </c>
       <c r="C670" s="1" t="s">
-        <v>1728</v>
+        <v>1724</v>
       </c>
       <c r="D670" s="1" t="s">
-        <v>1727</v>
+        <v>1725</v>
       </c>
     </row>
     <row r="671" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -15855,10 +15867,10 @@
         <v>1726</v>
       </c>
       <c r="B671" t="s">
-        <v>1729</v>
+        <v>129</v>
       </c>
       <c r="C671" s="1" t="s">
-        <v>1729</v>
+        <v>129</v>
       </c>
       <c r="D671" s="1" t="s">
         <v>1727</v>
@@ -15869,10 +15881,10 @@
         <v>1726</v>
       </c>
       <c r="B672" t="s">
-        <v>131</v>
+        <v>1728</v>
       </c>
       <c r="C672" s="1" t="s">
-        <v>131</v>
+        <v>1728</v>
       </c>
       <c r="D672" s="1" t="s">
         <v>1727</v>
@@ -15883,10 +15895,10 @@
         <v>1726</v>
       </c>
       <c r="B673" t="s">
-        <v>1730</v>
+        <v>1729</v>
       </c>
       <c r="C673" s="1" t="s">
-        <v>1730</v>
+        <v>1729</v>
       </c>
       <c r="D673" s="1" t="s">
         <v>1727</v>
@@ -15897,10 +15909,10 @@
         <v>1726</v>
       </c>
       <c r="B674" t="s">
-        <v>1488</v>
+        <v>131</v>
       </c>
       <c r="C674" s="1" t="s">
-        <v>1488</v>
+        <v>131</v>
       </c>
       <c r="D674" s="1" t="s">
         <v>1727</v>
@@ -15911,10 +15923,10 @@
         <v>1726</v>
       </c>
       <c r="B675" t="s">
-        <v>1731</v>
+        <v>1730</v>
       </c>
       <c r="C675" s="1" t="s">
-        <v>1731</v>
+        <v>1730</v>
       </c>
       <c r="D675" s="1" t="s">
         <v>1727</v>
@@ -15925,10 +15937,10 @@
         <v>1726</v>
       </c>
       <c r="B676" t="s">
-        <v>1732</v>
+        <v>1488</v>
       </c>
       <c r="C676" s="1" t="s">
-        <v>1732</v>
+        <v>1488</v>
       </c>
       <c r="D676" s="1" t="s">
         <v>1727</v>
@@ -15939,10 +15951,10 @@
         <v>1726</v>
       </c>
       <c r="B677" t="s">
-        <v>1733</v>
+        <v>1731</v>
       </c>
       <c r="C677" s="1" t="s">
-        <v>1733</v>
+        <v>1731</v>
       </c>
       <c r="D677" s="1" t="s">
         <v>1727</v>
@@ -15953,10 +15965,10 @@
         <v>1726</v>
       </c>
       <c r="B678" t="s">
-        <v>1734</v>
+        <v>1732</v>
       </c>
       <c r="C678" s="1" t="s">
-        <v>1734</v>
+        <v>1732</v>
       </c>
       <c r="D678" s="1" t="s">
         <v>1727</v>
@@ -15967,10 +15979,10 @@
         <v>1726</v>
       </c>
       <c r="B679" t="s">
-        <v>1735</v>
+        <v>1733</v>
       </c>
       <c r="C679" s="1" t="s">
-        <v>1735</v>
+        <v>1733</v>
       </c>
       <c r="D679" s="1" t="s">
         <v>1727</v>
@@ -15981,10 +15993,10 @@
         <v>1726</v>
       </c>
       <c r="B680" t="s">
-        <v>1736</v>
+        <v>1734</v>
       </c>
       <c r="C680" s="1" t="s">
-        <v>1736</v>
+        <v>1734</v>
       </c>
       <c r="D680" s="1" t="s">
         <v>1727</v>
@@ -15995,10 +16007,10 @@
         <v>1726</v>
       </c>
       <c r="B681" t="s">
-        <v>1737</v>
+        <v>1735</v>
       </c>
       <c r="C681" s="1" t="s">
-        <v>1737</v>
+        <v>1735</v>
       </c>
       <c r="D681" s="1" t="s">
         <v>1727</v>
@@ -16009,10 +16021,10 @@
         <v>1726</v>
       </c>
       <c r="B682" t="s">
-        <v>1738</v>
+        <v>1736</v>
       </c>
       <c r="C682" s="1" t="s">
-        <v>1738</v>
+        <v>1736</v>
       </c>
       <c r="D682" s="1" t="s">
         <v>1727</v>
@@ -16023,10 +16035,10 @@
         <v>1726</v>
       </c>
       <c r="B683" t="s">
-        <v>1739</v>
+        <v>1737</v>
       </c>
       <c r="C683" s="1" t="s">
-        <v>1739</v>
+        <v>1737</v>
       </c>
       <c r="D683" s="1" t="s">
         <v>1727</v>
@@ -16034,30 +16046,30 @@
     </row>
     <row r="684" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A684" t="s">
-        <v>1740</v>
+        <v>1726</v>
       </c>
       <c r="B684" t="s">
-        <v>1741</v>
+        <v>1738</v>
       </c>
       <c r="C684" s="1" t="s">
-        <v>1741</v>
+        <v>1738</v>
       </c>
       <c r="D684" s="1" t="s">
-        <v>1742</v>
+        <v>1727</v>
       </c>
     </row>
     <row r="685" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A685" t="s">
-        <v>1740</v>
+        <v>1726</v>
       </c>
       <c r="B685" t="s">
-        <v>1743</v>
+        <v>1739</v>
       </c>
       <c r="C685" s="1" t="s">
-        <v>1743</v>
+        <v>1739</v>
       </c>
       <c r="D685" s="1" t="s">
-        <v>1742</v>
+        <v>1727</v>
       </c>
     </row>
     <row r="686" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -16065,10 +16077,10 @@
         <v>1740</v>
       </c>
       <c r="B686" t="s">
-        <v>1744</v>
+        <v>1741</v>
       </c>
       <c r="C686" s="1" t="s">
-        <v>1744</v>
+        <v>1741</v>
       </c>
       <c r="D686" s="1" t="s">
         <v>1742</v>
@@ -16079,10 +16091,10 @@
         <v>1740</v>
       </c>
       <c r="B687" t="s">
-        <v>1745</v>
+        <v>1743</v>
       </c>
       <c r="C687" s="1" t="s">
-        <v>1745</v>
+        <v>1743</v>
       </c>
       <c r="D687" s="1" t="s">
         <v>1742</v>
@@ -16090,86 +16102,86 @@
     </row>
     <row r="688" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A688" t="s">
-        <v>1746</v>
+        <v>1740</v>
       </c>
       <c r="B688" t="s">
-        <v>1747</v>
+        <v>1744</v>
       </c>
       <c r="C688" s="1" t="s">
-        <v>1747</v>
+        <v>1744</v>
       </c>
       <c r="D688" s="1" t="s">
-        <v>1748</v>
+        <v>1742</v>
       </c>
     </row>
     <row r="689" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A689" t="s">
+        <v>1740</v>
+      </c>
+      <c r="B689" t="s">
+        <v>1745</v>
+      </c>
+      <c r="C689" s="1" t="s">
+        <v>1745</v>
+      </c>
+      <c r="D689" s="1" t="s">
+        <v>1742</v>
+      </c>
+    </row>
+    <row r="690" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A690" t="s">
         <v>1746</v>
       </c>
-      <c r="B689" t="s">
+      <c r="B690" t="s">
+        <v>1747</v>
+      </c>
+      <c r="C690" s="1" t="s">
+        <v>1747</v>
+      </c>
+      <c r="D690" s="1" t="s">
+        <v>1748</v>
+      </c>
+    </row>
+    <row r="691" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A691" t="s">
+        <v>1746</v>
+      </c>
+      <c r="B691" t="s">
         <v>1749</v>
       </c>
-      <c r="C689" s="1" t="s">
+      <c r="C691" s="1" t="s">
         <v>1749</v>
       </c>
-      <c r="D689" s="1" t="s">
+      <c r="D691" s="1" t="s">
         <v>1748</v>
       </c>
     </row>
-    <row r="690" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A690" t="s">
+    <row r="692" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A692" t="s">
         <v>1750</v>
       </c>
-      <c r="B690" t="s">
+      <c r="B692" t="s">
         <v>1751</v>
       </c>
-      <c r="C690" s="1" t="s">
+      <c r="C692" s="1" t="s">
         <v>1751</v>
       </c>
-      <c r="D690" s="1" t="s">
+      <c r="D692" s="1" t="s">
         <v>1752</v>
       </c>
     </row>
-    <row r="691" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A691" t="s">
+    <row r="693" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A693" t="s">
         <v>1750</v>
       </c>
-      <c r="B691" t="s">
+      <c r="B693" t="s">
         <v>1753</v>
       </c>
-      <c r="C691" s="1" t="s">
+      <c r="C693" s="1" t="s">
         <v>1753</v>
       </c>
-      <c r="D691" s="1" t="s">
+      <c r="D693" s="1" t="s">
         <v>1752</v>
-      </c>
-    </row>
-    <row r="692" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A692" t="s">
-        <v>1754</v>
-      </c>
-      <c r="B692" t="s">
-        <v>1755</v>
-      </c>
-      <c r="C692" s="1" t="s">
-        <v>1755</v>
-      </c>
-      <c r="D692" s="1" t="s">
-        <v>1756</v>
-      </c>
-    </row>
-    <row r="693" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A693" t="s">
-        <v>1754</v>
-      </c>
-      <c r="B693" t="s">
-        <v>1757</v>
-      </c>
-      <c r="C693" s="1" t="s">
-        <v>1757</v>
-      </c>
-      <c r="D693" s="1" t="s">
-        <v>1756</v>
       </c>
     </row>
     <row r="694" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -16177,10 +16189,10 @@
         <v>1754</v>
       </c>
       <c r="B694" t="s">
-        <v>1758</v>
+        <v>1755</v>
       </c>
       <c r="C694" s="1" t="s">
-        <v>1758</v>
+        <v>1755</v>
       </c>
       <c r="D694" s="1" t="s">
         <v>1756</v>
@@ -16191,10 +16203,10 @@
         <v>1754</v>
       </c>
       <c r="B695" t="s">
-        <v>1759</v>
+        <v>1757</v>
       </c>
       <c r="C695" s="1" t="s">
-        <v>1759</v>
+        <v>1757</v>
       </c>
       <c r="D695" s="1" t="s">
         <v>1756</v>
@@ -16205,10 +16217,10 @@
         <v>1754</v>
       </c>
       <c r="B696" t="s">
-        <v>1760</v>
+        <v>1758</v>
       </c>
       <c r="C696" s="1" t="s">
-        <v>1760</v>
+        <v>1758</v>
       </c>
       <c r="D696" s="1" t="s">
         <v>1756</v>
@@ -16219,10 +16231,10 @@
         <v>1754</v>
       </c>
       <c r="B697" t="s">
-        <v>1761</v>
+        <v>1759</v>
       </c>
       <c r="C697" s="1" t="s">
-        <v>1761</v>
+        <v>1759</v>
       </c>
       <c r="D697" s="1" t="s">
         <v>1756</v>
@@ -16233,10 +16245,10 @@
         <v>1754</v>
       </c>
       <c r="B698" t="s">
-        <v>1762</v>
+        <v>1760</v>
       </c>
       <c r="C698" s="1" t="s">
-        <v>1762</v>
+        <v>1760</v>
       </c>
       <c r="D698" s="1" t="s">
         <v>1756</v>
@@ -16244,30 +16256,30 @@
     </row>
     <row r="699" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A699" t="s">
-        <v>1763</v>
+        <v>1754</v>
       </c>
       <c r="B699" t="s">
-        <v>1764</v>
+        <v>1761</v>
       </c>
       <c r="C699" s="1" t="s">
-        <v>1765</v>
+        <v>1761</v>
       </c>
       <c r="D699" s="1" t="s">
-        <v>1766</v>
+        <v>1756</v>
       </c>
     </row>
     <row r="700" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A700" t="s">
-        <v>1763</v>
+        <v>1754</v>
       </c>
       <c r="B700" t="s">
-        <v>1767</v>
+        <v>1762</v>
       </c>
       <c r="C700" s="1" t="s">
-        <v>1768</v>
+        <v>1762</v>
       </c>
       <c r="D700" s="1" t="s">
-        <v>1769</v>
+        <v>1756</v>
       </c>
     </row>
     <row r="701" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -16275,41 +16287,41 @@
         <v>1763</v>
       </c>
       <c r="B701" t="s">
-        <v>1770</v>
+        <v>1764</v>
       </c>
       <c r="C701" s="1" t="s">
-        <v>1771</v>
+        <v>1765</v>
       </c>
       <c r="D701" s="1" t="s">
-        <v>1772</v>
+        <v>1766</v>
       </c>
     </row>
     <row r="702" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A702" t="s">
-        <v>1773</v>
+        <v>1763</v>
       </c>
       <c r="B702" t="s">
-        <v>1774</v>
+        <v>1767</v>
       </c>
       <c r="C702" s="1" t="s">
-        <v>1654</v>
+        <v>1768</v>
       </c>
       <c r="D702" s="1" t="s">
-        <v>1775</v>
+        <v>1769</v>
       </c>
     </row>
     <row r="703" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A703" t="s">
-        <v>1773</v>
+        <v>1763</v>
       </c>
       <c r="B703" t="s">
-        <v>1776</v>
+        <v>1770</v>
       </c>
       <c r="C703" s="1" t="s">
-        <v>1656</v>
+        <v>1771</v>
       </c>
       <c r="D703" s="1" t="s">
-        <v>1777</v>
+        <v>1772</v>
       </c>
     </row>
     <row r="704" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -16317,83 +16329,83 @@
         <v>1773</v>
       </c>
       <c r="B704" t="s">
-        <v>1778</v>
+        <v>1774</v>
       </c>
       <c r="C704" s="1" t="s">
-        <v>1779</v>
+        <v>1654</v>
       </c>
       <c r="D704" s="1" t="s">
-        <v>1780</v>
+        <v>1775</v>
       </c>
     </row>
     <row r="705" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A705" t="s">
-        <v>1781</v>
+        <v>1773</v>
       </c>
       <c r="B705" t="s">
-        <v>1782</v>
+        <v>1776</v>
       </c>
       <c r="C705" s="1" t="s">
-        <v>1782</v>
+        <v>1656</v>
       </c>
       <c r="D705" s="1" t="s">
-        <v>1783</v>
+        <v>1777</v>
       </c>
     </row>
     <row r="706" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A706" t="s">
-        <v>1781</v>
+        <v>1773</v>
       </c>
       <c r="B706" t="s">
-        <v>1784</v>
+        <v>1778</v>
       </c>
       <c r="C706" s="1" t="s">
-        <v>1784</v>
+        <v>1779</v>
       </c>
       <c r="D706" s="1" t="s">
-        <v>1783</v>
+        <v>1780</v>
       </c>
     </row>
     <row r="707" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A707" t="s">
-        <v>1785</v>
+        <v>1781</v>
       </c>
       <c r="B707" t="s">
-        <v>1786</v>
+        <v>1782</v>
       </c>
       <c r="C707" s="1" t="s">
-        <v>1786</v>
+        <v>1782</v>
       </c>
       <c r="D707" s="1" t="s">
-        <v>1787</v>
+        <v>1783</v>
       </c>
     </row>
     <row r="708" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A708" t="s">
-        <v>1788</v>
+        <v>1781</v>
       </c>
       <c r="B708" t="s">
-        <v>1789</v>
+        <v>1784</v>
       </c>
       <c r="C708" s="1" t="s">
-        <v>1789</v>
+        <v>1784</v>
       </c>
       <c r="D708" s="1" t="s">
-        <v>1790</v>
+        <v>1783</v>
       </c>
     </row>
     <row r="709" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A709" t="s">
-        <v>1788</v>
+        <v>1785</v>
       </c>
       <c r="B709" t="s">
-        <v>1791</v>
+        <v>1786</v>
       </c>
       <c r="C709" s="1" t="s">
-        <v>1791</v>
+        <v>1786</v>
       </c>
       <c r="D709" s="1" t="s">
-        <v>1790</v>
+        <v>1787</v>
       </c>
     </row>
     <row r="710" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -16401,10 +16413,10 @@
         <v>1788</v>
       </c>
       <c r="B710" t="s">
-        <v>1792</v>
+        <v>1789</v>
       </c>
       <c r="C710" s="1" t="s">
-        <v>1792</v>
+        <v>1789</v>
       </c>
       <c r="D710" s="1" t="s">
         <v>1790</v>
@@ -16412,29 +16424,57 @@
     </row>
     <row r="711" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A711" t="s">
-        <v>1793</v>
+        <v>1788</v>
       </c>
       <c r="B711" t="s">
-        <v>1794</v>
+        <v>1791</v>
       </c>
       <c r="C711" s="1" t="s">
-        <v>1794</v>
+        <v>1791</v>
       </c>
       <c r="D711" s="1" t="s">
-        <v>1795</v>
+        <v>1790</v>
       </c>
     </row>
     <row r="712" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A712" t="s">
+        <v>1788</v>
+      </c>
+      <c r="B712" t="s">
+        <v>1792</v>
+      </c>
+      <c r="C712" s="1" t="s">
+        <v>1792</v>
+      </c>
+      <c r="D712" s="1" t="s">
+        <v>1790</v>
+      </c>
+    </row>
+    <row r="713" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A713" t="s">
         <v>1793</v>
       </c>
-      <c r="B712" t="s">
+      <c r="B713" t="s">
+        <v>1794</v>
+      </c>
+      <c r="C713" s="1" t="s">
+        <v>1794</v>
+      </c>
+      <c r="D713" s="1" t="s">
+        <v>1795</v>
+      </c>
+    </row>
+    <row r="714" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A714" t="s">
+        <v>1793</v>
+      </c>
+      <c r="B714" t="s">
         <v>1796</v>
       </c>
-      <c r="C712" s="1" t="s">
+      <c r="C714" s="1" t="s">
         <v>1796</v>
       </c>
-      <c r="D712" s="1" t="s">
+      <c r="D714" s="1" t="s">
         <v>1795</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added values to OBInternalStatementInterestType1Code
Added UK.OBIE.InstalmentPlan and UK.OBIE.MoneyTransfer  to OBInternalStatementInterestType1Code
</commit_message>
<xml_diff>
--- a/OB_Internal_Codeset.xlsx
+++ b/OB_Internal_Codeset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/GitHub-repos/External_Internal_CodeSets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{074894BE-1596-9E4C-888B-8DF0AFA996E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A567A961-509F-B340-AAC9-D0CACB5AC00F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="34560" windowHeight="19820" xr2:uid="{4BA74A73-F883-C94E-AE65-527FEAB24FBE}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2842" uniqueCount="1801">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2850" uniqueCount="1803">
   <si>
     <t>Code Set</t>
   </si>
@@ -5502,6 +5502,12 @@
   </si>
   <si>
     <t>Returned payment fees charged during the statement period.</t>
+  </si>
+  <si>
+    <t>Interest on instalment plan</t>
+  </si>
+  <si>
+    <t>Interest on money transfers</t>
   </si>
 </sst>
 </file>
@@ -6060,8 +6066,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FFFB267F-52FF-2549-863C-D165F57A28C3}" name="Table1" displayName="Table1" ref="A1:F714" totalsRowShown="0">
-  <autoFilter ref="A1:F714" xr:uid="{FFFB267F-52FF-2549-863C-D165F57A28C3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FFFB267F-52FF-2549-863C-D165F57A28C3}" name="Table1" displayName="Table1" ref="A1:F716" totalsRowShown="0">
+  <autoFilter ref="A1:F716" xr:uid="{FFFB267F-52FF-2549-863C-D165F57A28C3}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{23F53907-045A-2545-8FDE-B8095E843B7C}" name="Code Set"/>
     <tableColumn id="2" xr3:uid="{8D12A497-C96F-094C-9D20-C8F6648FDFDB}" name="Code Value"/>
@@ -6391,10 +6397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EB901B9-ECA3-B946-8761-40B7A833F7F4}">
-  <dimension ref="A1:F714"/>
+  <dimension ref="A1:F716"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A481" workbookViewId="0">
-      <selection activeCell="A486" sqref="A486"/>
+    <sheetView tabSelected="1" topLeftCell="A483" workbookViewId="0">
+      <selection activeCell="D513" sqref="D513"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13666,30 +13672,30 @@
     </row>
     <row r="514" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A514" t="s">
-        <v>1404</v>
+        <v>1395</v>
       </c>
       <c r="B514" t="s">
-        <v>1405</v>
+        <v>1797</v>
       </c>
       <c r="C514" s="1" t="s">
-        <v>1405</v>
+        <v>1797</v>
       </c>
       <c r="D514" s="1" t="s">
-        <v>1406</v>
+        <v>1801</v>
       </c>
     </row>
     <row r="515" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A515" t="s">
-        <v>1404</v>
+        <v>1395</v>
       </c>
       <c r="B515" t="s">
-        <v>1407</v>
+        <v>1381</v>
       </c>
       <c r="C515" s="1" t="s">
-        <v>1407</v>
+        <v>1381</v>
       </c>
       <c r="D515" s="1" t="s">
-        <v>1408</v>
+        <v>1802</v>
       </c>
     </row>
     <row r="516" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -13697,13 +13703,13 @@
         <v>1404</v>
       </c>
       <c r="B516" t="s">
-        <v>1409</v>
+        <v>1405</v>
       </c>
       <c r="C516" s="1" t="s">
-        <v>1409</v>
+        <v>1405</v>
       </c>
       <c r="D516" s="1" t="s">
-        <v>1410</v>
+        <v>1406</v>
       </c>
     </row>
     <row r="517" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -13711,13 +13717,13 @@
         <v>1404</v>
       </c>
       <c r="B517" t="s">
-        <v>1411</v>
+        <v>1407</v>
       </c>
       <c r="C517" s="1" t="s">
-        <v>1411</v>
+        <v>1407</v>
       </c>
       <c r="D517" s="1" t="s">
-        <v>1412</v>
+        <v>1408</v>
       </c>
     </row>
     <row r="518" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -13725,13 +13731,13 @@
         <v>1404</v>
       </c>
       <c r="B518" t="s">
-        <v>1413</v>
+        <v>1409</v>
       </c>
       <c r="C518" s="1" t="s">
-        <v>1413</v>
+        <v>1409</v>
       </c>
       <c r="D518" s="1" t="s">
-        <v>1414</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="519" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -13739,13 +13745,13 @@
         <v>1404</v>
       </c>
       <c r="B519" t="s">
-        <v>1415</v>
+        <v>1411</v>
       </c>
       <c r="C519" s="1" t="s">
-        <v>1415</v>
+        <v>1411</v>
       </c>
       <c r="D519" s="1" t="s">
-        <v>1416</v>
+        <v>1412</v>
       </c>
     </row>
     <row r="520" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -13753,13 +13759,13 @@
         <v>1404</v>
       </c>
       <c r="B520" t="s">
-        <v>1417</v>
+        <v>1413</v>
       </c>
       <c r="C520" s="1" t="s">
-        <v>1417</v>
+        <v>1413</v>
       </c>
       <c r="D520" s="1" t="s">
-        <v>1418</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="521" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -13767,13 +13773,13 @@
         <v>1404</v>
       </c>
       <c r="B521" t="s">
-        <v>1419</v>
+        <v>1415</v>
       </c>
       <c r="C521" s="1" t="s">
-        <v>1419</v>
+        <v>1415</v>
       </c>
       <c r="D521" s="1" t="s">
-        <v>1420</v>
+        <v>1416</v>
       </c>
     </row>
     <row r="522" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -13781,13 +13787,13 @@
         <v>1404</v>
       </c>
       <c r="B522" t="s">
-        <v>1421</v>
+        <v>1417</v>
       </c>
       <c r="C522" s="1" t="s">
-        <v>1421</v>
+        <v>1417</v>
       </c>
       <c r="D522" s="1" t="s">
-        <v>1422</v>
+        <v>1418</v>
       </c>
     </row>
     <row r="523" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -13795,41 +13801,41 @@
         <v>1404</v>
       </c>
       <c r="B523" t="s">
-        <v>1423</v>
+        <v>1419</v>
       </c>
       <c r="C523" s="1" t="s">
-        <v>1423</v>
+        <v>1419</v>
       </c>
       <c r="D523" s="1" t="s">
-        <v>1424</v>
+        <v>1420</v>
       </c>
     </row>
     <row r="524" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A524" t="s">
-        <v>1425</v>
+        <v>1404</v>
       </c>
       <c r="B524" t="s">
-        <v>1426</v>
+        <v>1421</v>
       </c>
       <c r="C524" s="1" t="s">
-        <v>1426</v>
+        <v>1421</v>
       </c>
       <c r="D524" s="1" t="s">
-        <v>1427</v>
+        <v>1422</v>
       </c>
     </row>
     <row r="525" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A525" t="s">
-        <v>1425</v>
+        <v>1404</v>
       </c>
       <c r="B525" t="s">
-        <v>1428</v>
+        <v>1423</v>
       </c>
       <c r="C525" s="1" t="s">
-        <v>1428</v>
+        <v>1423</v>
       </c>
       <c r="D525" s="1" t="s">
-        <v>1427</v>
+        <v>1424</v>
       </c>
     </row>
     <row r="526" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -13837,13 +13843,13 @@
         <v>1425</v>
       </c>
       <c r="B526" t="s">
-        <v>1429</v>
+        <v>1426</v>
       </c>
       <c r="C526" s="1" t="s">
-        <v>1429</v>
+        <v>1426</v>
       </c>
       <c r="D526" s="1" t="s">
-        <v>1430</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="527" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -13851,13 +13857,13 @@
         <v>1425</v>
       </c>
       <c r="B527" t="s">
-        <v>1431</v>
+        <v>1428</v>
       </c>
       <c r="C527" s="1" t="s">
-        <v>1431</v>
+        <v>1428</v>
       </c>
       <c r="D527" s="1" t="s">
-        <v>1432</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="528" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -13865,13 +13871,13 @@
         <v>1425</v>
       </c>
       <c r="B528" t="s">
-        <v>1433</v>
+        <v>1429</v>
       </c>
       <c r="C528" s="1" t="s">
-        <v>1433</v>
+        <v>1429</v>
       </c>
       <c r="D528" s="1" t="s">
-        <v>1434</v>
+        <v>1430</v>
       </c>
     </row>
     <row r="529" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -13879,13 +13885,13 @@
         <v>1425</v>
       </c>
       <c r="B529" t="s">
-        <v>1435</v>
+        <v>1431</v>
       </c>
       <c r="C529" s="1" t="s">
-        <v>1435</v>
+        <v>1431</v>
       </c>
       <c r="D529" s="1" t="s">
-        <v>1434</v>
+        <v>1432</v>
       </c>
     </row>
     <row r="530" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -13893,13 +13899,13 @@
         <v>1425</v>
       </c>
       <c r="B530" t="s">
-        <v>1436</v>
+        <v>1433</v>
       </c>
       <c r="C530" s="1" t="s">
-        <v>1436</v>
+        <v>1433</v>
       </c>
       <c r="D530" s="1" t="s">
-        <v>1437</v>
+        <v>1434</v>
       </c>
     </row>
     <row r="531" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -13907,69 +13913,69 @@
         <v>1425</v>
       </c>
       <c r="B531" t="s">
+        <v>1435</v>
+      </c>
+      <c r="C531" s="1" t="s">
+        <v>1435</v>
+      </c>
+      <c r="D531" s="1" t="s">
+        <v>1434</v>
+      </c>
+    </row>
+    <row r="532" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A532" t="s">
+        <v>1425</v>
+      </c>
+      <c r="B532" t="s">
+        <v>1436</v>
+      </c>
+      <c r="C532" s="1" t="s">
+        <v>1436</v>
+      </c>
+      <c r="D532" s="1" t="s">
+        <v>1437</v>
+      </c>
+    </row>
+    <row r="533" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A533" t="s">
+        <v>1425</v>
+      </c>
+      <c r="B533" t="s">
         <v>1438</v>
       </c>
-      <c r="C531" s="1" t="s">
+      <c r="C533" s="1" t="s">
         <v>1438</v>
       </c>
-      <c r="D531" s="1" t="s">
+      <c r="D533" s="1" t="s">
         <v>1437</v>
       </c>
     </row>
-    <row r="532" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A532" t="s">
+    <row r="534" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A534" t="s">
         <v>1439</v>
       </c>
-      <c r="B532" t="s">
+      <c r="B534" t="s">
         <v>1440</v>
       </c>
-      <c r="C532" s="1" t="s">
+      <c r="C534" s="1" t="s">
         <v>1440</v>
       </c>
-      <c r="D532" s="1" t="s">
+      <c r="D534" s="1" t="s">
         <v>1441</v>
       </c>
     </row>
-    <row r="533" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A533" t="s">
+    <row r="535" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A535" t="s">
         <v>1439</v>
       </c>
-      <c r="B533" t="s">
+      <c r="B535" t="s">
         <v>1442</v>
       </c>
-      <c r="C533" s="1" t="s">
+      <c r="C535" s="1" t="s">
         <v>1442</v>
       </c>
-      <c r="D533" s="1" t="s">
+      <c r="D535" s="1" t="s">
         <v>1443</v>
-      </c>
-    </row>
-    <row r="534" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A534" t="s">
-        <v>1444</v>
-      </c>
-      <c r="B534" t="s">
-        <v>1445</v>
-      </c>
-      <c r="C534" s="1" t="s">
-        <v>1445</v>
-      </c>
-      <c r="D534" s="1" t="s">
-        <v>1446</v>
-      </c>
-    </row>
-    <row r="535" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A535" t="s">
-        <v>1444</v>
-      </c>
-      <c r="B535" t="s">
-        <v>1447</v>
-      </c>
-      <c r="C535" s="1" t="s">
-        <v>1447</v>
-      </c>
-      <c r="D535" s="1" t="s">
-        <v>1448</v>
       </c>
     </row>
     <row r="536" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -13977,13 +13983,13 @@
         <v>1444</v>
       </c>
       <c r="B536" t="s">
-        <v>1449</v>
+        <v>1445</v>
       </c>
       <c r="C536" s="1" t="s">
-        <v>1449</v>
+        <v>1445</v>
       </c>
       <c r="D536" s="1" t="s">
-        <v>1450</v>
+        <v>1446</v>
       </c>
     </row>
     <row r="537" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -13991,13 +13997,13 @@
         <v>1444</v>
       </c>
       <c r="B537" t="s">
-        <v>1451</v>
+        <v>1447</v>
       </c>
       <c r="C537" s="1" t="s">
-        <v>1451</v>
+        <v>1447</v>
       </c>
       <c r="D537" s="1" t="s">
-        <v>1452</v>
+        <v>1448</v>
       </c>
     </row>
     <row r="538" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14005,13 +14011,13 @@
         <v>1444</v>
       </c>
       <c r="B538" t="s">
-        <v>1453</v>
+        <v>1449</v>
       </c>
       <c r="C538" s="1" t="s">
-        <v>1453</v>
+        <v>1449</v>
       </c>
       <c r="D538" s="1" t="s">
-        <v>1454</v>
+        <v>1450</v>
       </c>
     </row>
     <row r="539" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14019,55 +14025,55 @@
         <v>1444</v>
       </c>
       <c r="B539" t="s">
-        <v>1455</v>
+        <v>1451</v>
       </c>
       <c r="C539" s="1" t="s">
-        <v>1455</v>
+        <v>1451</v>
       </c>
       <c r="D539" s="1" t="s">
-        <v>1456</v>
-      </c>
-    </row>
-    <row r="540" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>1452</v>
+      </c>
+    </row>
+    <row r="540" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A540" t="s">
-        <v>1457</v>
+        <v>1444</v>
       </c>
       <c r="B540" t="s">
-        <v>1458</v>
+        <v>1453</v>
       </c>
       <c r="C540" s="1" t="s">
-        <v>1458</v>
+        <v>1453</v>
       </c>
       <c r="D540" s="1" t="s">
-        <v>1459</v>
+        <v>1454</v>
       </c>
     </row>
     <row r="541" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A541" t="s">
-        <v>1457</v>
+        <v>1444</v>
       </c>
       <c r="B541" t="s">
-        <v>1460</v>
+        <v>1455</v>
       </c>
       <c r="C541" s="1" t="s">
-        <v>1460</v>
+        <v>1455</v>
       </c>
       <c r="D541" s="1" t="s">
-        <v>1461</v>
-      </c>
-    </row>
-    <row r="542" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>1456</v>
+      </c>
+    </row>
+    <row r="542" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A542" t="s">
         <v>1457</v>
       </c>
       <c r="B542" t="s">
-        <v>1462</v>
+        <v>1458</v>
       </c>
       <c r="C542" s="1" t="s">
-        <v>1462</v>
+        <v>1458</v>
       </c>
       <c r="D542" s="1" t="s">
-        <v>1463</v>
+        <v>1459</v>
       </c>
     </row>
     <row r="543" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14075,13 +14081,13 @@
         <v>1457</v>
       </c>
       <c r="B543" t="s">
-        <v>1464</v>
+        <v>1460</v>
       </c>
       <c r="C543" s="1" t="s">
-        <v>1464</v>
+        <v>1460</v>
       </c>
       <c r="D543" s="1" t="s">
-        <v>1465</v>
+        <v>1461</v>
       </c>
     </row>
     <row r="544" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14089,41 +14095,41 @@
         <v>1457</v>
       </c>
       <c r="B544" t="s">
-        <v>1466</v>
+        <v>1462</v>
       </c>
       <c r="C544" s="1" t="s">
-        <v>1466</v>
+        <v>1462</v>
       </c>
       <c r="D544" s="1" t="s">
-        <v>1467</v>
+        <v>1463</v>
       </c>
     </row>
     <row r="545" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A545" t="s">
-        <v>1468</v>
+        <v>1457</v>
       </c>
       <c r="B545" t="s">
-        <v>1469</v>
+        <v>1464</v>
       </c>
       <c r="C545" s="1" t="s">
-        <v>1469</v>
+        <v>1464</v>
       </c>
       <c r="D545" s="1" t="s">
-        <v>1470</v>
+        <v>1465</v>
       </c>
     </row>
     <row r="546" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A546" t="s">
-        <v>1468</v>
+        <v>1457</v>
       </c>
       <c r="B546" t="s">
-        <v>1471</v>
+        <v>1466</v>
       </c>
       <c r="C546" s="1" t="s">
-        <v>1471</v>
+        <v>1466</v>
       </c>
       <c r="D546" s="1" t="s">
-        <v>1472</v>
+        <v>1467</v>
       </c>
     </row>
     <row r="547" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14131,13 +14137,13 @@
         <v>1468</v>
       </c>
       <c r="B547" t="s">
-        <v>1383</v>
+        <v>1469</v>
       </c>
       <c r="C547" s="1" t="s">
-        <v>1383</v>
+        <v>1469</v>
       </c>
       <c r="D547" s="1" t="s">
-        <v>1473</v>
+        <v>1470</v>
       </c>
     </row>
     <row r="548" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14145,13 +14151,13 @@
         <v>1468</v>
       </c>
       <c r="B548" t="s">
-        <v>1474</v>
+        <v>1471</v>
       </c>
       <c r="C548" s="1" t="s">
-        <v>1474</v>
+        <v>1471</v>
       </c>
       <c r="D548" s="1" t="s">
-        <v>1475</v>
+        <v>1472</v>
       </c>
     </row>
     <row r="549" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14159,13 +14165,13 @@
         <v>1468</v>
       </c>
       <c r="B549" t="s">
-        <v>1453</v>
+        <v>1383</v>
       </c>
       <c r="C549" s="1" t="s">
-        <v>1453</v>
+        <v>1383</v>
       </c>
       <c r="D549" s="1" t="s">
-        <v>1454</v>
+        <v>1473</v>
       </c>
     </row>
     <row r="550" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14173,13 +14179,13 @@
         <v>1468</v>
       </c>
       <c r="B550" t="s">
-        <v>1455</v>
+        <v>1474</v>
       </c>
       <c r="C550" s="1" t="s">
-        <v>1455</v>
+        <v>1474</v>
       </c>
       <c r="D550" s="1" t="s">
-        <v>1456</v>
+        <v>1475</v>
       </c>
     </row>
     <row r="551" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14187,41 +14193,41 @@
         <v>1468</v>
       </c>
       <c r="B551" t="s">
-        <v>1476</v>
+        <v>1453</v>
       </c>
       <c r="C551" s="1" t="s">
-        <v>1476</v>
+        <v>1453</v>
       </c>
       <c r="D551" s="1" t="s">
-        <v>1477</v>
+        <v>1454</v>
       </c>
     </row>
     <row r="552" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A552" t="s">
-        <v>1478</v>
+        <v>1468</v>
       </c>
       <c r="B552" t="s">
-        <v>1479</v>
+        <v>1455</v>
       </c>
       <c r="C552" s="1" t="s">
-        <v>1479</v>
+        <v>1455</v>
       </c>
       <c r="D552" s="1" t="s">
-        <v>1480</v>
+        <v>1456</v>
       </c>
     </row>
     <row r="553" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A553" t="s">
-        <v>1478</v>
+        <v>1468</v>
       </c>
       <c r="B553" t="s">
-        <v>1481</v>
+        <v>1476</v>
       </c>
       <c r="C553" s="1" t="s">
-        <v>1481</v>
+        <v>1476</v>
       </c>
       <c r="D553" s="1" t="s">
-        <v>1482</v>
+        <v>1477</v>
       </c>
     </row>
     <row r="554" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14229,13 +14235,13 @@
         <v>1478</v>
       </c>
       <c r="B554" t="s">
-        <v>1483</v>
+        <v>1479</v>
       </c>
       <c r="C554" s="1" t="s">
-        <v>1483</v>
+        <v>1479</v>
       </c>
       <c r="D554" s="1" t="s">
-        <v>1484</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="555" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14243,13 +14249,13 @@
         <v>1478</v>
       </c>
       <c r="B555" t="s">
-        <v>1485</v>
+        <v>1481</v>
       </c>
       <c r="C555" s="1" t="s">
-        <v>1485</v>
+        <v>1481</v>
       </c>
       <c r="D555" s="1" t="s">
-        <v>1486</v>
+        <v>1482</v>
       </c>
     </row>
     <row r="556" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14257,13 +14263,13 @@
         <v>1478</v>
       </c>
       <c r="B556" t="s">
-        <v>1487</v>
+        <v>1483</v>
       </c>
       <c r="C556" s="1" t="s">
-        <v>1487</v>
+        <v>1483</v>
       </c>
       <c r="D556" s="1" t="s">
-        <v>1488</v>
+        <v>1484</v>
       </c>
     </row>
     <row r="557" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14271,13 +14277,13 @@
         <v>1478</v>
       </c>
       <c r="B557" t="s">
-        <v>1489</v>
+        <v>1485</v>
       </c>
       <c r="C557" s="1" t="s">
-        <v>1489</v>
+        <v>1485</v>
       </c>
       <c r="D557" s="1" t="s">
-        <v>1490</v>
+        <v>1486</v>
       </c>
     </row>
     <row r="558" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14285,13 +14291,13 @@
         <v>1478</v>
       </c>
       <c r="B558" t="s">
-        <v>1491</v>
+        <v>1487</v>
       </c>
       <c r="C558" s="1" t="s">
-        <v>1491</v>
+        <v>1487</v>
       </c>
       <c r="D558" s="1" t="s">
-        <v>1492</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="559" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14299,13 +14305,13 @@
         <v>1478</v>
       </c>
       <c r="B559" t="s">
-        <v>1493</v>
+        <v>1489</v>
       </c>
       <c r="C559" s="1" t="s">
-        <v>1493</v>
+        <v>1489</v>
       </c>
       <c r="D559" s="1" t="s">
-        <v>1494</v>
+        <v>1490</v>
       </c>
     </row>
     <row r="560" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14313,13 +14319,13 @@
         <v>1478</v>
       </c>
       <c r="B560" t="s">
-        <v>1495</v>
+        <v>1491</v>
       </c>
       <c r="C560" s="1" t="s">
-        <v>1495</v>
+        <v>1491</v>
       </c>
       <c r="D560" s="1" t="s">
-        <v>1496</v>
+        <v>1492</v>
       </c>
     </row>
     <row r="561" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14327,13 +14333,13 @@
         <v>1478</v>
       </c>
       <c r="B561" t="s">
-        <v>1497</v>
+        <v>1493</v>
       </c>
       <c r="C561" s="1" t="s">
-        <v>1497</v>
+        <v>1493</v>
       </c>
       <c r="D561" s="1" t="s">
-        <v>1498</v>
+        <v>1494</v>
       </c>
     </row>
     <row r="562" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14341,13 +14347,13 @@
         <v>1478</v>
       </c>
       <c r="B562" t="s">
-        <v>1499</v>
+        <v>1495</v>
       </c>
       <c r="C562" s="1" t="s">
-        <v>1499</v>
+        <v>1495</v>
       </c>
       <c r="D562" s="1" t="s">
-        <v>1500</v>
+        <v>1496</v>
       </c>
     </row>
     <row r="563" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14355,41 +14361,41 @@
         <v>1478</v>
       </c>
       <c r="B563" t="s">
-        <v>1501</v>
+        <v>1497</v>
       </c>
       <c r="C563" s="1" t="s">
-        <v>1501</v>
+        <v>1497</v>
       </c>
       <c r="D563" s="1" t="s">
-        <v>1502</v>
+        <v>1498</v>
       </c>
     </row>
     <row r="564" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A564" t="s">
-        <v>1503</v>
+        <v>1478</v>
       </c>
       <c r="B564" t="s">
-        <v>1504</v>
+        <v>1499</v>
       </c>
       <c r="C564" s="1" t="s">
-        <v>1504</v>
+        <v>1499</v>
       </c>
       <c r="D564" s="1" t="s">
-        <v>1505</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="565" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A565" t="s">
-        <v>1503</v>
+        <v>1478</v>
       </c>
       <c r="B565" t="s">
-        <v>1506</v>
+        <v>1501</v>
       </c>
       <c r="C565" s="1" t="s">
-        <v>1506</v>
+        <v>1501</v>
       </c>
       <c r="D565" s="1" t="s">
-        <v>1507</v>
+        <v>1502</v>
       </c>
     </row>
     <row r="566" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14397,13 +14403,13 @@
         <v>1503</v>
       </c>
       <c r="B566" t="s">
-        <v>1508</v>
+        <v>1504</v>
       </c>
       <c r="C566" s="1" t="s">
-        <v>1508</v>
+        <v>1504</v>
       </c>
       <c r="D566" s="1" t="s">
-        <v>1509</v>
+        <v>1505</v>
       </c>
     </row>
     <row r="567" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14411,13 +14417,13 @@
         <v>1503</v>
       </c>
       <c r="B567" t="s">
-        <v>1510</v>
+        <v>1506</v>
       </c>
       <c r="C567" s="1" t="s">
-        <v>1510</v>
+        <v>1506</v>
       </c>
       <c r="D567" s="1" t="s">
-        <v>1511</v>
+        <v>1507</v>
       </c>
     </row>
     <row r="568" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14425,13 +14431,13 @@
         <v>1503</v>
       </c>
       <c r="B568" t="s">
-        <v>1512</v>
+        <v>1508</v>
       </c>
       <c r="C568" s="1" t="s">
-        <v>1512</v>
+        <v>1508</v>
       </c>
       <c r="D568" s="1" t="s">
-        <v>1513</v>
+        <v>1509</v>
       </c>
     </row>
     <row r="569" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14439,13 +14445,13 @@
         <v>1503</v>
       </c>
       <c r="B569" t="s">
-        <v>1514</v>
+        <v>1510</v>
       </c>
       <c r="C569" s="1" t="s">
-        <v>1514</v>
+        <v>1510</v>
       </c>
       <c r="D569" s="1" t="s">
-        <v>1515</v>
+        <v>1511</v>
       </c>
     </row>
     <row r="570" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14453,13 +14459,13 @@
         <v>1503</v>
       </c>
       <c r="B570" t="s">
-        <v>1516</v>
+        <v>1512</v>
       </c>
       <c r="C570" s="1" t="s">
-        <v>1516</v>
+        <v>1512</v>
       </c>
       <c r="D570" s="1" t="s">
-        <v>1517</v>
+        <v>1513</v>
       </c>
     </row>
     <row r="571" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14467,13 +14473,13 @@
         <v>1503</v>
       </c>
       <c r="B571" t="s">
-        <v>1518</v>
+        <v>1514</v>
       </c>
       <c r="C571" s="1" t="s">
-        <v>1518</v>
+        <v>1514</v>
       </c>
       <c r="D571" s="1" t="s">
-        <v>1519</v>
+        <v>1515</v>
       </c>
     </row>
     <row r="572" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14481,13 +14487,13 @@
         <v>1503</v>
       </c>
       <c r="B572" t="s">
-        <v>1520</v>
+        <v>1516</v>
       </c>
       <c r="C572" s="1" t="s">
-        <v>1520</v>
+        <v>1516</v>
       </c>
       <c r="D572" s="1" t="s">
-        <v>1521</v>
+        <v>1517</v>
       </c>
     </row>
     <row r="573" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14495,13 +14501,13 @@
         <v>1503</v>
       </c>
       <c r="B573" t="s">
-        <v>1522</v>
+        <v>1518</v>
       </c>
       <c r="C573" s="1" t="s">
-        <v>1522</v>
+        <v>1518</v>
       </c>
       <c r="D573" s="1" t="s">
-        <v>1523</v>
+        <v>1519</v>
       </c>
     </row>
     <row r="574" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14509,13 +14515,13 @@
         <v>1503</v>
       </c>
       <c r="B574" t="s">
-        <v>1524</v>
+        <v>1520</v>
       </c>
       <c r="C574" s="1" t="s">
-        <v>1524</v>
+        <v>1520</v>
       </c>
       <c r="D574" s="1" t="s">
-        <v>1525</v>
+        <v>1521</v>
       </c>
     </row>
     <row r="575" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14523,13 +14529,13 @@
         <v>1503</v>
       </c>
       <c r="B575" t="s">
-        <v>1526</v>
+        <v>1522</v>
       </c>
       <c r="C575" s="1" t="s">
-        <v>1526</v>
+        <v>1522</v>
       </c>
       <c r="D575" s="1" t="s">
-        <v>1527</v>
+        <v>1523</v>
       </c>
     </row>
     <row r="576" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14537,13 +14543,13 @@
         <v>1503</v>
       </c>
       <c r="B576" t="s">
-        <v>1528</v>
+        <v>1524</v>
       </c>
       <c r="C576" s="1" t="s">
-        <v>1528</v>
+        <v>1524</v>
       </c>
       <c r="D576" s="1" t="s">
-        <v>1529</v>
+        <v>1525</v>
       </c>
     </row>
     <row r="577" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14551,69 +14557,69 @@
         <v>1503</v>
       </c>
       <c r="B577" t="s">
-        <v>1530</v>
+        <v>1526</v>
       </c>
       <c r="C577" s="1" t="s">
-        <v>1530</v>
+        <v>1526</v>
       </c>
       <c r="D577" s="1" t="s">
-        <v>1531</v>
+        <v>1527</v>
       </c>
     </row>
     <row r="578" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A578" t="s">
-        <v>1532</v>
+        <v>1503</v>
       </c>
       <c r="B578" t="s">
-        <v>1533</v>
+        <v>1528</v>
       </c>
       <c r="C578" s="1" t="s">
-        <v>1533</v>
+        <v>1528</v>
       </c>
       <c r="D578" s="1" t="s">
-        <v>1534</v>
+        <v>1529</v>
       </c>
     </row>
     <row r="579" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A579" t="s">
-        <v>1532</v>
+        <v>1503</v>
       </c>
       <c r="B579" t="s">
-        <v>1535</v>
+        <v>1530</v>
       </c>
       <c r="C579" s="1" t="s">
-        <v>1535</v>
+        <v>1530</v>
       </c>
       <c r="D579" s="1" t="s">
-        <v>1536</v>
+        <v>1531</v>
       </c>
     </row>
     <row r="580" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A580" t="s">
-        <v>1537</v>
+        <v>1532</v>
       </c>
       <c r="B580" t="s">
-        <v>1538</v>
+        <v>1533</v>
       </c>
       <c r="C580" s="1" t="s">
-        <v>1538</v>
+        <v>1533</v>
       </c>
       <c r="D580" s="1" t="s">
-        <v>1539</v>
+        <v>1534</v>
       </c>
     </row>
     <row r="581" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A581" t="s">
-        <v>1537</v>
+        <v>1532</v>
       </c>
       <c r="B581" t="s">
-        <v>1540</v>
+        <v>1535</v>
       </c>
       <c r="C581" s="1" t="s">
-        <v>1540</v>
+        <v>1535</v>
       </c>
       <c r="D581" s="1" t="s">
-        <v>1541</v>
+        <v>1536</v>
       </c>
     </row>
     <row r="582" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14621,13 +14627,13 @@
         <v>1537</v>
       </c>
       <c r="B582" t="s">
-        <v>1542</v>
+        <v>1538</v>
       </c>
       <c r="C582" s="1" t="s">
-        <v>1542</v>
+        <v>1538</v>
       </c>
       <c r="D582" s="1" t="s">
-        <v>1543</v>
+        <v>1539</v>
       </c>
     </row>
     <row r="583" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14635,13 +14641,13 @@
         <v>1537</v>
       </c>
       <c r="B583" t="s">
-        <v>1544</v>
+        <v>1540</v>
       </c>
       <c r="C583" s="1" t="s">
-        <v>1544</v>
+        <v>1540</v>
       </c>
       <c r="D583" s="1" t="s">
-        <v>1545</v>
+        <v>1541</v>
       </c>
     </row>
     <row r="584" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14649,13 +14655,13 @@
         <v>1537</v>
       </c>
       <c r="B584" t="s">
-        <v>1367</v>
+        <v>1542</v>
       </c>
       <c r="C584" s="1" t="s">
-        <v>1367</v>
+        <v>1542</v>
       </c>
       <c r="D584" s="1" t="s">
-        <v>1546</v>
+        <v>1543</v>
       </c>
     </row>
     <row r="585" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14663,13 +14669,13 @@
         <v>1537</v>
       </c>
       <c r="B585" t="s">
-        <v>1381</v>
+        <v>1544</v>
       </c>
       <c r="C585" s="1" t="s">
-        <v>1381</v>
+        <v>1544</v>
       </c>
       <c r="D585" s="1" t="s">
-        <v>1547</v>
+        <v>1545</v>
       </c>
     </row>
     <row r="586" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14677,13 +14683,13 @@
         <v>1537</v>
       </c>
       <c r="B586" t="s">
-        <v>1278</v>
+        <v>1367</v>
       </c>
       <c r="C586" s="1" t="s">
-        <v>1278</v>
+        <v>1367</v>
       </c>
       <c r="D586" s="1" t="s">
-        <v>1548</v>
+        <v>1546</v>
       </c>
     </row>
     <row r="587" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14691,13 +14697,13 @@
         <v>1537</v>
       </c>
       <c r="B587" t="s">
-        <v>1549</v>
+        <v>1381</v>
       </c>
       <c r="C587" s="1" t="s">
-        <v>1549</v>
+        <v>1381</v>
       </c>
       <c r="D587" s="1" t="s">
-        <v>1550</v>
+        <v>1547</v>
       </c>
     </row>
     <row r="588" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14705,13 +14711,13 @@
         <v>1537</v>
       </c>
       <c r="B588" t="s">
-        <v>1551</v>
+        <v>1278</v>
       </c>
       <c r="C588" s="1" t="s">
-        <v>1551</v>
+        <v>1278</v>
       </c>
       <c r="D588" s="1" t="s">
-        <v>1552</v>
+        <v>1548</v>
       </c>
     </row>
     <row r="589" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14719,13 +14725,13 @@
         <v>1537</v>
       </c>
       <c r="B589" t="s">
-        <v>1553</v>
+        <v>1549</v>
       </c>
       <c r="C589" s="1" t="s">
-        <v>1553</v>
+        <v>1549</v>
       </c>
       <c r="D589" s="1" t="s">
-        <v>1554</v>
+        <v>1550</v>
       </c>
     </row>
     <row r="590" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14733,13 +14739,13 @@
         <v>1537</v>
       </c>
       <c r="B590" t="s">
-        <v>1555</v>
+        <v>1551</v>
       </c>
       <c r="C590" s="1" t="s">
-        <v>1555</v>
+        <v>1551</v>
       </c>
       <c r="D590" s="1" t="s">
-        <v>1556</v>
+        <v>1552</v>
       </c>
     </row>
     <row r="591" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14747,41 +14753,41 @@
         <v>1537</v>
       </c>
       <c r="B591" t="s">
-        <v>1557</v>
+        <v>1553</v>
       </c>
       <c r="C591" s="1" t="s">
-        <v>1557</v>
+        <v>1553</v>
       </c>
       <c r="D591" s="1" t="s">
-        <v>1558</v>
+        <v>1554</v>
       </c>
     </row>
     <row r="592" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A592" t="s">
-        <v>1559</v>
+        <v>1537</v>
       </c>
       <c r="B592" t="s">
-        <v>1560</v>
+        <v>1555</v>
       </c>
       <c r="C592" s="1" t="s">
-        <v>1560</v>
+        <v>1555</v>
       </c>
       <c r="D592" s="1" t="s">
-        <v>1561</v>
+        <v>1556</v>
       </c>
     </row>
     <row r="593" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A593" t="s">
-        <v>1559</v>
+        <v>1537</v>
       </c>
       <c r="B593" t="s">
-        <v>1562</v>
+        <v>1557</v>
       </c>
       <c r="C593" s="1" t="s">
-        <v>1562</v>
+        <v>1557</v>
       </c>
       <c r="D593" s="1" t="s">
-        <v>1563</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="594" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14789,69 +14795,69 @@
         <v>1559</v>
       </c>
       <c r="B594" t="s">
-        <v>1564</v>
+        <v>1560</v>
       </c>
       <c r="C594" s="1" t="s">
-        <v>1564</v>
+        <v>1560</v>
       </c>
       <c r="D594" s="1" t="s">
-        <v>1565</v>
+        <v>1561</v>
       </c>
     </row>
     <row r="595" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A595" t="s">
-        <v>1566</v>
+        <v>1559</v>
       </c>
       <c r="B595" t="s">
-        <v>1567</v>
+        <v>1562</v>
       </c>
       <c r="C595" s="1" t="s">
-        <v>1567</v>
+        <v>1562</v>
       </c>
       <c r="D595" s="1" t="s">
-        <v>1568</v>
-      </c>
-    </row>
-    <row r="596" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>1563</v>
+      </c>
+    </row>
+    <row r="596" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A596" t="s">
-        <v>1566</v>
+        <v>1559</v>
       </c>
       <c r="B596" t="s">
-        <v>1569</v>
+        <v>1564</v>
       </c>
       <c r="C596" s="1" t="s">
-        <v>1569</v>
+        <v>1564</v>
       </c>
       <c r="D596" s="1" t="s">
-        <v>1570</v>
+        <v>1565</v>
       </c>
     </row>
     <row r="597" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A597" t="s">
-        <v>1571</v>
+        <v>1566</v>
       </c>
       <c r="B597" t="s">
-        <v>1572</v>
+        <v>1567</v>
       </c>
       <c r="C597" s="1" t="s">
-        <v>1572</v>
+        <v>1567</v>
       </c>
       <c r="D597" s="1" t="s">
-        <v>1573</v>
-      </c>
-    </row>
-    <row r="598" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>1568</v>
+      </c>
+    </row>
+    <row r="598" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A598" t="s">
-        <v>1571</v>
+        <v>1566</v>
       </c>
       <c r="B598" t="s">
-        <v>1574</v>
+        <v>1569</v>
       </c>
       <c r="C598" s="1" t="s">
-        <v>1574</v>
+        <v>1569</v>
       </c>
       <c r="D598" s="1" t="s">
-        <v>1575</v>
+        <v>1570</v>
       </c>
     </row>
     <row r="599" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -14859,167 +14865,167 @@
         <v>1571</v>
       </c>
       <c r="B599" t="s">
-        <v>1576</v>
+        <v>1572</v>
       </c>
       <c r="C599" s="1" t="s">
-        <v>1576</v>
+        <v>1572</v>
       </c>
       <c r="D599" s="1" t="s">
-        <v>1577</v>
-      </c>
-    </row>
-    <row r="600" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>1573</v>
+      </c>
+    </row>
+    <row r="600" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A600" t="s">
         <v>1571</v>
       </c>
       <c r="B600" t="s">
-        <v>1578</v>
+        <v>1574</v>
       </c>
       <c r="C600" s="1" t="s">
-        <v>1578</v>
+        <v>1574</v>
       </c>
       <c r="D600" s="1" t="s">
-        <v>1579</v>
+        <v>1575</v>
       </c>
     </row>
     <row r="601" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A601" t="s">
-        <v>1580</v>
+        <v>1571</v>
       </c>
       <c r="B601" t="s">
-        <v>1581</v>
+        <v>1576</v>
       </c>
       <c r="C601" s="1" t="s">
-        <v>1581</v>
+        <v>1576</v>
       </c>
       <c r="D601" s="1" t="s">
-        <v>1582</v>
+        <v>1577</v>
       </c>
     </row>
     <row r="602" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A602" t="s">
-        <v>1580</v>
+        <v>1571</v>
       </c>
       <c r="B602" t="s">
-        <v>1583</v>
+        <v>1578</v>
       </c>
       <c r="C602" s="1" t="s">
-        <v>1583</v>
+        <v>1578</v>
       </c>
       <c r="D602" s="1" t="s">
-        <v>1584</v>
+        <v>1579</v>
       </c>
     </row>
     <row r="603" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A603" t="s">
-        <v>1585</v>
+        <v>1580</v>
       </c>
       <c r="B603" t="s">
-        <v>1586</v>
+        <v>1581</v>
       </c>
       <c r="C603" s="1" t="s">
-        <v>1586</v>
+        <v>1581</v>
       </c>
       <c r="D603" s="1" t="s">
-        <v>1587</v>
-      </c>
-    </row>
-    <row r="604" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>1582</v>
+      </c>
+    </row>
+    <row r="604" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A604" t="s">
-        <v>1585</v>
+        <v>1580</v>
       </c>
       <c r="B604" t="s">
-        <v>1588</v>
+        <v>1583</v>
       </c>
       <c r="C604" s="1" t="s">
-        <v>1588</v>
+        <v>1583</v>
       </c>
       <c r="D604" s="1" t="s">
-        <v>1589</v>
+        <v>1584</v>
       </c>
     </row>
     <row r="605" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A605" t="s">
-        <v>1590</v>
+        <v>1585</v>
       </c>
       <c r="B605" t="s">
-        <v>1591</v>
+        <v>1586</v>
       </c>
       <c r="C605" s="1" t="s">
-        <v>1591</v>
+        <v>1586</v>
       </c>
       <c r="D605" s="1" t="s">
-        <v>1592</v>
-      </c>
-    </row>
-    <row r="606" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>1587</v>
+      </c>
+    </row>
+    <row r="606" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A606" t="s">
-        <v>1590</v>
+        <v>1585</v>
       </c>
       <c r="B606" t="s">
-        <v>1593</v>
+        <v>1588</v>
       </c>
       <c r="C606" s="1" t="s">
-        <v>1593</v>
+        <v>1588</v>
       </c>
       <c r="D606" s="1" t="s">
-        <v>1594</v>
+        <v>1589</v>
       </c>
     </row>
     <row r="607" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A607" t="s">
-        <v>1595</v>
+        <v>1590</v>
       </c>
       <c r="B607" t="s">
-        <v>1596</v>
+        <v>1591</v>
       </c>
       <c r="C607" s="1" t="s">
-        <v>1596</v>
+        <v>1591</v>
       </c>
       <c r="D607" s="1" t="s">
-        <v>1597</v>
-      </c>
-    </row>
-    <row r="608" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>1592</v>
+      </c>
+    </row>
+    <row r="608" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A608" t="s">
-        <v>1595</v>
+        <v>1590</v>
       </c>
       <c r="B608" t="s">
-        <v>1598</v>
+        <v>1593</v>
       </c>
       <c r="C608" s="1" t="s">
-        <v>1598</v>
+        <v>1593</v>
       </c>
       <c r="D608" s="1" t="s">
-        <v>1599</v>
+        <v>1594</v>
       </c>
     </row>
     <row r="609" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A609" t="s">
-        <v>1600</v>
+        <v>1595</v>
       </c>
       <c r="B609" t="s">
-        <v>1601</v>
+        <v>1596</v>
       </c>
       <c r="C609" s="1" t="s">
-        <v>1601</v>
+        <v>1596</v>
       </c>
       <c r="D609" s="1" t="s">
-        <v>1602</v>
-      </c>
-    </row>
-    <row r="610" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>1597</v>
+      </c>
+    </row>
+    <row r="610" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A610" t="s">
-        <v>1600</v>
+        <v>1595</v>
       </c>
       <c r="B610" t="s">
-        <v>1603</v>
+        <v>1598</v>
       </c>
       <c r="C610" s="1" t="s">
-        <v>1603</v>
+        <v>1598</v>
       </c>
       <c r="D610" s="1" t="s">
-        <v>1604</v>
+        <v>1599</v>
       </c>
     </row>
     <row r="611" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -15027,41 +15033,41 @@
         <v>1600</v>
       </c>
       <c r="B611" t="s">
-        <v>1605</v>
+        <v>1601</v>
       </c>
       <c r="C611" s="1" t="s">
-        <v>1605</v>
+        <v>1601</v>
       </c>
       <c r="D611" s="1" t="s">
-        <v>1606</v>
-      </c>
-    </row>
-    <row r="612" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>1602</v>
+      </c>
+    </row>
+    <row r="612" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A612" t="s">
         <v>1600</v>
       </c>
       <c r="B612" t="s">
-        <v>1607</v>
+        <v>1603</v>
       </c>
       <c r="C612" s="1" t="s">
-        <v>1607</v>
+        <v>1603</v>
       </c>
       <c r="D612" s="1" t="s">
-        <v>1608</v>
-      </c>
-    </row>
-    <row r="613" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>1604</v>
+      </c>
+    </row>
+    <row r="613" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A613" t="s">
         <v>1600</v>
       </c>
       <c r="B613" t="s">
-        <v>1609</v>
+        <v>1605</v>
       </c>
       <c r="C613" s="1" t="s">
-        <v>1609</v>
+        <v>1605</v>
       </c>
       <c r="D613" s="1" t="s">
-        <v>1610</v>
+        <v>1606</v>
       </c>
     </row>
     <row r="614" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -15069,41 +15075,41 @@
         <v>1600</v>
       </c>
       <c r="B614" t="s">
-        <v>1611</v>
+        <v>1607</v>
       </c>
       <c r="C614" s="1" t="s">
-        <v>1611</v>
+        <v>1607</v>
       </c>
       <c r="D614" s="1" t="s">
-        <v>1612</v>
-      </c>
-    </row>
-    <row r="615" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>1608</v>
+      </c>
+    </row>
+    <row r="615" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A615" t="s">
         <v>1600</v>
       </c>
       <c r="B615" t="s">
-        <v>1613</v>
+        <v>1609</v>
       </c>
       <c r="C615" s="1" t="s">
-        <v>1613</v>
+        <v>1609</v>
       </c>
       <c r="D615" s="1" t="s">
-        <v>1614</v>
-      </c>
-    </row>
-    <row r="616" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>1610</v>
+      </c>
+    </row>
+    <row r="616" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A616" t="s">
         <v>1600</v>
       </c>
       <c r="B616" t="s">
-        <v>1615</v>
+        <v>1611</v>
       </c>
       <c r="C616" s="1" t="s">
-        <v>1615</v>
+        <v>1611</v>
       </c>
       <c r="D616" s="1" t="s">
-        <v>1616</v>
+        <v>1612</v>
       </c>
     </row>
     <row r="617" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -15111,27 +15117,27 @@
         <v>1600</v>
       </c>
       <c r="B617" t="s">
-        <v>1617</v>
+        <v>1613</v>
       </c>
       <c r="C617" s="1" t="s">
-        <v>1617</v>
+        <v>1613</v>
       </c>
       <c r="D617" s="1" t="s">
-        <v>1618</v>
-      </c>
-    </row>
-    <row r="618" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>1614</v>
+      </c>
+    </row>
+    <row r="618" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A618" t="s">
         <v>1600</v>
       </c>
       <c r="B618" t="s">
-        <v>1619</v>
+        <v>1615</v>
       </c>
       <c r="C618" s="1" t="s">
-        <v>1619</v>
+        <v>1615</v>
       </c>
       <c r="D618" s="1" t="s">
-        <v>1620</v>
+        <v>1616</v>
       </c>
     </row>
     <row r="619" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -15139,13 +15145,13 @@
         <v>1600</v>
       </c>
       <c r="B619" t="s">
-        <v>1621</v>
+        <v>1617</v>
       </c>
       <c r="C619" s="1" t="s">
-        <v>1621</v>
+        <v>1617</v>
       </c>
       <c r="D619" s="1" t="s">
-        <v>1622</v>
+        <v>1618</v>
       </c>
     </row>
     <row r="620" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -15153,13 +15159,13 @@
         <v>1600</v>
       </c>
       <c r="B620" t="s">
-        <v>1623</v>
+        <v>1619</v>
       </c>
       <c r="C620" s="1" t="s">
-        <v>1623</v>
+        <v>1619</v>
       </c>
       <c r="D620" s="1" t="s">
-        <v>1624</v>
+        <v>1620</v>
       </c>
     </row>
     <row r="621" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -15167,13 +15173,13 @@
         <v>1600</v>
       </c>
       <c r="B621" t="s">
-        <v>1625</v>
+        <v>1621</v>
       </c>
       <c r="C621" s="1" t="s">
-        <v>1625</v>
+        <v>1621</v>
       </c>
       <c r="D621" s="1" t="s">
-        <v>1626</v>
+        <v>1622</v>
       </c>
     </row>
     <row r="622" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -15181,13 +15187,13 @@
         <v>1600</v>
       </c>
       <c r="B622" t="s">
-        <v>1627</v>
+        <v>1623</v>
       </c>
       <c r="C622" s="1" t="s">
-        <v>1627</v>
+        <v>1623</v>
       </c>
       <c r="D622" s="1" t="s">
-        <v>1628</v>
+        <v>1624</v>
       </c>
     </row>
     <row r="623" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -15195,13 +15201,13 @@
         <v>1600</v>
       </c>
       <c r="B623" t="s">
-        <v>1629</v>
+        <v>1625</v>
       </c>
       <c r="C623" s="1" t="s">
-        <v>1629</v>
+        <v>1625</v>
       </c>
       <c r="D623" s="1" t="s">
-        <v>1630</v>
+        <v>1626</v>
       </c>
     </row>
     <row r="624" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -15209,69 +15215,69 @@
         <v>1600</v>
       </c>
       <c r="B624" t="s">
-        <v>1631</v>
+        <v>1627</v>
       </c>
       <c r="C624" s="1" t="s">
-        <v>1631</v>
+        <v>1627</v>
       </c>
       <c r="D624" s="1" t="s">
-        <v>1632</v>
-      </c>
-    </row>
-    <row r="625" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+        <v>1628</v>
+      </c>
+    </row>
+    <row r="625" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A625" t="s">
         <v>1600</v>
       </c>
       <c r="B625" t="s">
-        <v>1633</v>
+        <v>1629</v>
       </c>
       <c r="C625" s="1" t="s">
-        <v>1633</v>
+        <v>1629</v>
       </c>
       <c r="D625" s="1" t="s">
-        <v>1634</v>
-      </c>
-    </row>
-    <row r="626" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+        <v>1630</v>
+      </c>
+    </row>
+    <row r="626" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A626" t="s">
         <v>1600</v>
       </c>
       <c r="B626" t="s">
-        <v>1635</v>
+        <v>1631</v>
       </c>
       <c r="C626" s="1" t="s">
-        <v>1635</v>
+        <v>1631</v>
       </c>
       <c r="D626" s="1" t="s">
-        <v>1636</v>
-      </c>
-    </row>
-    <row r="627" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+        <v>1632</v>
+      </c>
+    </row>
+    <row r="627" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A627" t="s">
         <v>1600</v>
       </c>
       <c r="B627" t="s">
-        <v>1637</v>
+        <v>1633</v>
       </c>
       <c r="C627" s="1" t="s">
-        <v>1637</v>
+        <v>1633</v>
       </c>
       <c r="D627" s="1" t="s">
-        <v>1638</v>
-      </c>
-    </row>
-    <row r="628" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+        <v>1634</v>
+      </c>
+    </row>
+    <row r="628" spans="1:4" ht="68" x14ac:dyDescent="0.2">
       <c r="A628" t="s">
         <v>1600</v>
       </c>
       <c r="B628" t="s">
-        <v>1639</v>
+        <v>1635</v>
       </c>
       <c r="C628" s="1" t="s">
-        <v>1639</v>
+        <v>1635</v>
       </c>
       <c r="D628" s="1" t="s">
-        <v>1640</v>
+        <v>1636</v>
       </c>
     </row>
     <row r="629" spans="1:4" ht="85" x14ac:dyDescent="0.2">
@@ -15279,41 +15285,41 @@
         <v>1600</v>
       </c>
       <c r="B629" t="s">
+        <v>1637</v>
+      </c>
+      <c r="C629" s="1" t="s">
+        <v>1637</v>
+      </c>
+      <c r="D629" s="1" t="s">
+        <v>1638</v>
+      </c>
+    </row>
+    <row r="630" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A630" t="s">
+        <v>1600</v>
+      </c>
+      <c r="B630" t="s">
+        <v>1639</v>
+      </c>
+      <c r="C630" s="1" t="s">
+        <v>1639</v>
+      </c>
+      <c r="D630" s="1" t="s">
+        <v>1640</v>
+      </c>
+    </row>
+    <row r="631" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+      <c r="A631" t="s">
+        <v>1600</v>
+      </c>
+      <c r="B631" t="s">
         <v>1641</v>
       </c>
-      <c r="C629" s="1" t="s">
+      <c r="C631" s="1" t="s">
         <v>1641</v>
       </c>
-      <c r="D629" s="1" t="s">
+      <c r="D631" s="1" t="s">
         <v>1642</v>
-      </c>
-    </row>
-    <row r="630" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A630" t="s">
-        <v>1643</v>
-      </c>
-      <c r="B630" t="s">
-        <v>1644</v>
-      </c>
-      <c r="C630" s="1" t="s">
-        <v>1644</v>
-      </c>
-      <c r="D630" s="1" t="s">
-        <v>1645</v>
-      </c>
-    </row>
-    <row r="631" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A631" t="s">
-        <v>1643</v>
-      </c>
-      <c r="B631" t="s">
-        <v>1646</v>
-      </c>
-      <c r="C631" s="1" t="s">
-        <v>1646</v>
-      </c>
-      <c r="D631" s="1" t="s">
-        <v>1647</v>
       </c>
     </row>
     <row r="632" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -15321,27 +15327,27 @@
         <v>1643</v>
       </c>
       <c r="B632" t="s">
-        <v>1648</v>
+        <v>1644</v>
       </c>
       <c r="C632" s="1" t="s">
-        <v>1648</v>
+        <v>1644</v>
       </c>
       <c r="D632" s="1" t="s">
-        <v>1649</v>
-      </c>
-    </row>
-    <row r="633" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>1645</v>
+      </c>
+    </row>
+    <row r="633" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A633" t="s">
         <v>1643</v>
       </c>
       <c r="B633" t="s">
-        <v>1650</v>
+        <v>1646</v>
       </c>
       <c r="C633" s="1" t="s">
-        <v>1650</v>
+        <v>1646</v>
       </c>
       <c r="D633" s="1" t="s">
-        <v>1651</v>
+        <v>1647</v>
       </c>
     </row>
     <row r="634" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -15349,83 +15355,83 @@
         <v>1643</v>
       </c>
       <c r="B634" t="s">
-        <v>185</v>
+        <v>1648</v>
       </c>
       <c r="C634" s="1" t="s">
-        <v>185</v>
+        <v>1648</v>
       </c>
       <c r="D634" s="1" t="s">
-        <v>1652</v>
-      </c>
-    </row>
-    <row r="635" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>1649</v>
+      </c>
+    </row>
+    <row r="635" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A635" t="s">
-        <v>1653</v>
+        <v>1643</v>
       </c>
       <c r="B635" t="s">
-        <v>1654</v>
+        <v>1650</v>
       </c>
       <c r="C635" s="1" t="s">
-        <v>1654</v>
+        <v>1650</v>
       </c>
       <c r="D635" s="1" t="s">
-        <v>1655</v>
+        <v>1651</v>
       </c>
     </row>
     <row r="636" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A636" t="s">
-        <v>1653</v>
+        <v>1643</v>
       </c>
       <c r="B636" t="s">
-        <v>1656</v>
+        <v>185</v>
       </c>
       <c r="C636" s="1" t="s">
-        <v>1656</v>
+        <v>185</v>
       </c>
       <c r="D636" s="1" t="s">
-        <v>1657</v>
+        <v>1652</v>
       </c>
     </row>
     <row r="637" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A637" t="s">
-        <v>1658</v>
+        <v>1653</v>
       </c>
       <c r="B637" t="s">
-        <v>1659</v>
+        <v>1654</v>
       </c>
       <c r="C637" s="1" t="s">
-        <v>1660</v>
+        <v>1654</v>
       </c>
       <c r="D637" s="1" t="s">
-        <v>1661</v>
+        <v>1655</v>
       </c>
     </row>
     <row r="638" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A638" t="s">
-        <v>1658</v>
+        <v>1653</v>
       </c>
       <c r="B638" t="s">
-        <v>1654</v>
+        <v>1656</v>
       </c>
       <c r="C638" s="1" t="s">
-        <v>1654</v>
+        <v>1656</v>
       </c>
       <c r="D638" s="1" t="s">
-        <v>1662</v>
-      </c>
-    </row>
-    <row r="639" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+        <v>1657</v>
+      </c>
+    </row>
+    <row r="639" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A639" t="s">
         <v>1658</v>
       </c>
       <c r="B639" t="s">
-        <v>1663</v>
+        <v>1659</v>
       </c>
       <c r="C639" s="1" t="s">
-        <v>1663</v>
+        <v>1660</v>
       </c>
       <c r="D639" s="1" t="s">
-        <v>1664</v>
+        <v>1661</v>
       </c>
     </row>
     <row r="640" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -15433,83 +15439,83 @@
         <v>1658</v>
       </c>
       <c r="B640" t="s">
-        <v>1665</v>
+        <v>1654</v>
       </c>
       <c r="C640" s="1" t="s">
-        <v>1665</v>
+        <v>1654</v>
       </c>
       <c r="D640" s="1" t="s">
-        <v>1666</v>
-      </c>
-    </row>
-    <row r="641" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>1662</v>
+      </c>
+    </row>
+    <row r="641" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A641" t="s">
         <v>1658</v>
       </c>
       <c r="B641" t="s">
-        <v>1667</v>
+        <v>1663</v>
       </c>
       <c r="C641" s="1" t="s">
-        <v>1667</v>
+        <v>1663</v>
       </c>
       <c r="D641" s="1" t="s">
-        <v>1668</v>
+        <v>1664</v>
       </c>
     </row>
     <row r="642" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A642" t="s">
-        <v>1669</v>
+        <v>1658</v>
       </c>
       <c r="B642" t="s">
-        <v>1670</v>
+        <v>1665</v>
       </c>
       <c r="C642" s="1" t="s">
-        <v>1670</v>
+        <v>1665</v>
       </c>
       <c r="D642" s="1" t="s">
-        <v>1671</v>
+        <v>1666</v>
       </c>
     </row>
     <row r="643" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A643" t="s">
-        <v>1669</v>
+        <v>1658</v>
       </c>
       <c r="B643" t="s">
-        <v>1672</v>
+        <v>1667</v>
       </c>
       <c r="C643" s="1" t="s">
-        <v>1672</v>
+        <v>1667</v>
       </c>
       <c r="D643" s="1" t="s">
-        <v>1671</v>
+        <v>1668</v>
       </c>
     </row>
     <row r="644" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A644" t="s">
-        <v>1673</v>
+        <v>1669</v>
       </c>
       <c r="B644" t="s">
-        <v>1674</v>
+        <v>1670</v>
       </c>
       <c r="C644" s="1" t="s">
-        <v>1674</v>
+        <v>1670</v>
       </c>
       <c r="D644" s="1" t="s">
-        <v>1675</v>
+        <v>1671</v>
       </c>
     </row>
     <row r="645" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A645" t="s">
-        <v>1673</v>
+        <v>1669</v>
       </c>
       <c r="B645" t="s">
-        <v>1676</v>
+        <v>1672</v>
       </c>
       <c r="C645" s="1" t="s">
-        <v>1676</v>
+        <v>1672</v>
       </c>
       <c r="D645" s="1" t="s">
-        <v>1677</v>
+        <v>1671</v>
       </c>
     </row>
     <row r="646" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -15517,13 +15523,13 @@
         <v>1673</v>
       </c>
       <c r="B646" t="s">
-        <v>1678</v>
+        <v>1674</v>
       </c>
       <c r="C646" s="1" t="s">
-        <v>1678</v>
+        <v>1674</v>
       </c>
       <c r="D646" s="1" t="s">
-        <v>1679</v>
+        <v>1675</v>
       </c>
     </row>
     <row r="647" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -15531,13 +15537,13 @@
         <v>1673</v>
       </c>
       <c r="B647" t="s">
-        <v>1680</v>
+        <v>1676</v>
       </c>
       <c r="C647" s="1" t="s">
-        <v>1680</v>
+        <v>1676</v>
       </c>
       <c r="D647" s="1" t="s">
-        <v>1681</v>
+        <v>1677</v>
       </c>
     </row>
     <row r="648" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -15545,41 +15551,41 @@
         <v>1673</v>
       </c>
       <c r="B648" t="s">
-        <v>1682</v>
+        <v>1678</v>
       </c>
       <c r="C648" s="1" t="s">
-        <v>1682</v>
+        <v>1678</v>
       </c>
       <c r="D648" s="1" t="s">
-        <v>1683</v>
+        <v>1679</v>
       </c>
     </row>
     <row r="649" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A649" t="s">
-        <v>1684</v>
+        <v>1673</v>
       </c>
       <c r="B649" t="s">
-        <v>1685</v>
+        <v>1680</v>
       </c>
       <c r="C649" s="1" t="s">
-        <v>1685</v>
+        <v>1680</v>
       </c>
       <c r="D649" s="1" t="s">
-        <v>1686</v>
+        <v>1681</v>
       </c>
     </row>
     <row r="650" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A650" t="s">
-        <v>1684</v>
+        <v>1673</v>
       </c>
       <c r="B650" t="s">
-        <v>1687</v>
+        <v>1682</v>
       </c>
       <c r="C650" s="1" t="s">
-        <v>1687</v>
+        <v>1682</v>
       </c>
       <c r="D650" s="1" t="s">
-        <v>1688</v>
+        <v>1683</v>
       </c>
     </row>
     <row r="651" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -15587,13 +15593,13 @@
         <v>1684</v>
       </c>
       <c r="B651" t="s">
-        <v>1689</v>
+        <v>1685</v>
       </c>
       <c r="C651" s="1" t="s">
-        <v>1689</v>
+        <v>1685</v>
       </c>
       <c r="D651" s="1" t="s">
-        <v>1690</v>
+        <v>1686</v>
       </c>
     </row>
     <row r="652" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -15601,80 +15607,80 @@
         <v>1684</v>
       </c>
       <c r="B652" t="s">
-        <v>1691</v>
+        <v>1687</v>
       </c>
       <c r="C652" s="1" t="s">
-        <v>1691</v>
+        <v>1687</v>
       </c>
       <c r="D652" s="1" t="s">
-        <v>1692</v>
+        <v>1688</v>
       </c>
     </row>
     <row r="653" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A653" t="s">
-        <v>1693</v>
+        <v>1684</v>
       </c>
       <c r="B653" t="s">
-        <v>1694</v>
+        <v>1689</v>
       </c>
       <c r="C653" s="1" t="s">
-        <v>1694</v>
+        <v>1689</v>
       </c>
       <c r="D653" s="1" t="s">
-        <v>1695</v>
+        <v>1690</v>
       </c>
     </row>
     <row r="654" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A654" t="s">
+        <v>1684</v>
+      </c>
+      <c r="B654" t="s">
+        <v>1691</v>
+      </c>
+      <c r="C654" s="1" t="s">
+        <v>1691</v>
+      </c>
+      <c r="D654" s="1" t="s">
+        <v>1692</v>
+      </c>
+    </row>
+    <row r="655" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A655" t="s">
         <v>1693</v>
       </c>
-      <c r="B654" t="s">
+      <c r="B655" t="s">
+        <v>1694</v>
+      </c>
+      <c r="C655" s="1" t="s">
+        <v>1694</v>
+      </c>
+      <c r="D655" s="1" t="s">
+        <v>1695</v>
+      </c>
+    </row>
+    <row r="656" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A656" t="s">
+        <v>1693</v>
+      </c>
+      <c r="B656" t="s">
         <v>1696</v>
       </c>
-      <c r="C654" s="1" t="s">
+      <c r="C656" s="1" t="s">
         <v>1696</v>
       </c>
-      <c r="D654" s="1" t="s">
+      <c r="D656" s="1" t="s">
         <v>1695</v>
-      </c>
-    </row>
-    <row r="655" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A655" t="s">
-        <v>1673</v>
-      </c>
-      <c r="B655" t="s">
-        <v>1697</v>
-      </c>
-      <c r="C655" s="1" t="s">
-        <v>1697</v>
-      </c>
-      <c r="D655" s="1" t="s">
-        <v>1698</v>
-      </c>
-    </row>
-    <row r="656" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A656" t="s">
-        <v>1699</v>
-      </c>
-      <c r="B656" t="s">
-        <v>1700</v>
-      </c>
-      <c r="C656" s="1" t="s">
-        <v>1700</v>
-      </c>
-      <c r="D656" s="1" t="s">
-        <v>1698</v>
       </c>
     </row>
     <row r="657" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A657" t="s">
-        <v>1699</v>
+        <v>1673</v>
       </c>
       <c r="B657" t="s">
-        <v>318</v>
+        <v>1697</v>
       </c>
       <c r="C657" s="1" t="s">
-        <v>318</v>
+        <v>1697</v>
       </c>
       <c r="D657" s="1" t="s">
         <v>1698</v>
@@ -15685,10 +15691,10 @@
         <v>1699</v>
       </c>
       <c r="B658" t="s">
-        <v>1701</v>
+        <v>1700</v>
       </c>
       <c r="C658" s="1" t="s">
-        <v>1701</v>
+        <v>1700</v>
       </c>
       <c r="D658" s="1" t="s">
         <v>1698</v>
@@ -15699,10 +15705,10 @@
         <v>1699</v>
       </c>
       <c r="B659" t="s">
-        <v>1702</v>
+        <v>318</v>
       </c>
       <c r="C659" s="1" t="s">
-        <v>1702</v>
+        <v>318</v>
       </c>
       <c r="D659" s="1" t="s">
         <v>1698</v>
@@ -15713,41 +15719,41 @@
         <v>1699</v>
       </c>
       <c r="B660" t="s">
-        <v>1697</v>
+        <v>1701</v>
       </c>
       <c r="C660" s="1" t="s">
-        <v>1697</v>
+        <v>1701</v>
       </c>
       <c r="D660" s="1" t="s">
         <v>1698</v>
       </c>
     </row>
-    <row r="661" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="661" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A661" t="s">
-        <v>1703</v>
+        <v>1699</v>
       </c>
       <c r="B661" t="s">
-        <v>1704</v>
+        <v>1702</v>
       </c>
       <c r="C661" s="1" t="s">
-        <v>1704</v>
+        <v>1702</v>
       </c>
       <c r="D661" s="1" t="s">
-        <v>1705</v>
-      </c>
-    </row>
-    <row r="662" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>1698</v>
+      </c>
+    </row>
+    <row r="662" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A662" t="s">
-        <v>1703</v>
+        <v>1699</v>
       </c>
       <c r="B662" t="s">
-        <v>1706</v>
+        <v>1697</v>
       </c>
       <c r="C662" s="1" t="s">
-        <v>1706</v>
+        <v>1697</v>
       </c>
       <c r="D662" s="1" t="s">
-        <v>1707</v>
+        <v>1698</v>
       </c>
     </row>
     <row r="663" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -15755,69 +15761,69 @@
         <v>1703</v>
       </c>
       <c r="B663" t="s">
-        <v>1708</v>
+        <v>1704</v>
       </c>
       <c r="C663" s="1" t="s">
-        <v>1708</v>
+        <v>1704</v>
       </c>
       <c r="D663" s="1" t="s">
-        <v>1709</v>
+        <v>1705</v>
       </c>
     </row>
     <row r="664" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A664" t="s">
-        <v>1710</v>
+        <v>1703</v>
       </c>
       <c r="B664" t="s">
-        <v>1711</v>
+        <v>1706</v>
       </c>
       <c r="C664" s="1" t="s">
-        <v>1711</v>
+        <v>1706</v>
       </c>
       <c r="D664" s="1" t="s">
-        <v>1712</v>
+        <v>1707</v>
       </c>
     </row>
     <row r="665" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A665" t="s">
-        <v>1710</v>
+        <v>1703</v>
       </c>
       <c r="B665" t="s">
-        <v>1713</v>
+        <v>1708</v>
       </c>
       <c r="C665" s="1" t="s">
-        <v>1713</v>
+        <v>1708</v>
       </c>
       <c r="D665" s="1" t="s">
-        <v>1714</v>
+        <v>1709</v>
       </c>
     </row>
     <row r="666" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A666" t="s">
-        <v>1715</v>
+        <v>1710</v>
       </c>
       <c r="B666" t="s">
-        <v>1716</v>
+        <v>1711</v>
       </c>
       <c r="C666" s="1" t="s">
-        <v>1716</v>
+        <v>1711</v>
       </c>
       <c r="D666" s="1" t="s">
-        <v>1717</v>
+        <v>1712</v>
       </c>
     </row>
     <row r="667" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A667" t="s">
-        <v>1715</v>
+        <v>1710</v>
       </c>
       <c r="B667" t="s">
-        <v>1718</v>
+        <v>1713</v>
       </c>
       <c r="C667" s="1" t="s">
-        <v>1718</v>
+        <v>1713</v>
       </c>
       <c r="D667" s="1" t="s">
-        <v>1719</v>
+        <v>1714</v>
       </c>
     </row>
     <row r="668" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -15825,13 +15831,13 @@
         <v>1715</v>
       </c>
       <c r="B668" t="s">
-        <v>1720</v>
+        <v>1716</v>
       </c>
       <c r="C668" s="1" t="s">
-        <v>1720</v>
+        <v>1716</v>
       </c>
       <c r="D668" s="1" t="s">
-        <v>1721</v>
+        <v>1717</v>
       </c>
     </row>
     <row r="669" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -15839,13 +15845,13 @@
         <v>1715</v>
       </c>
       <c r="B669" t="s">
-        <v>1722</v>
+        <v>1718</v>
       </c>
       <c r="C669" s="1" t="s">
-        <v>1722</v>
+        <v>1718</v>
       </c>
       <c r="D669" s="1" t="s">
-        <v>1723</v>
+        <v>1719</v>
       </c>
     </row>
     <row r="670" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -15853,41 +15859,41 @@
         <v>1715</v>
       </c>
       <c r="B670" t="s">
-        <v>1724</v>
+        <v>1720</v>
       </c>
       <c r="C670" s="1" t="s">
-        <v>1724</v>
+        <v>1720</v>
       </c>
       <c r="D670" s="1" t="s">
-        <v>1725</v>
+        <v>1721</v>
       </c>
     </row>
     <row r="671" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A671" t="s">
-        <v>1726</v>
+        <v>1715</v>
       </c>
       <c r="B671" t="s">
-        <v>129</v>
+        <v>1722</v>
       </c>
       <c r="C671" s="1" t="s">
-        <v>129</v>
+        <v>1722</v>
       </c>
       <c r="D671" s="1" t="s">
-        <v>1727</v>
+        <v>1723</v>
       </c>
     </row>
     <row r="672" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A672" t="s">
-        <v>1726</v>
+        <v>1715</v>
       </c>
       <c r="B672" t="s">
-        <v>1728</v>
+        <v>1724</v>
       </c>
       <c r="C672" s="1" t="s">
-        <v>1728</v>
+        <v>1724</v>
       </c>
       <c r="D672" s="1" t="s">
-        <v>1727</v>
+        <v>1725</v>
       </c>
     </row>
     <row r="673" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -15895,10 +15901,10 @@
         <v>1726</v>
       </c>
       <c r="B673" t="s">
-        <v>1729</v>
+        <v>129</v>
       </c>
       <c r="C673" s="1" t="s">
-        <v>1729</v>
+        <v>129</v>
       </c>
       <c r="D673" s="1" t="s">
         <v>1727</v>
@@ -15909,10 +15915,10 @@
         <v>1726</v>
       </c>
       <c r="B674" t="s">
-        <v>131</v>
+        <v>1728</v>
       </c>
       <c r="C674" s="1" t="s">
-        <v>131</v>
+        <v>1728</v>
       </c>
       <c r="D674" s="1" t="s">
         <v>1727</v>
@@ -15923,10 +15929,10 @@
         <v>1726</v>
       </c>
       <c r="B675" t="s">
-        <v>1730</v>
+        <v>1729</v>
       </c>
       <c r="C675" s="1" t="s">
-        <v>1730</v>
+        <v>1729</v>
       </c>
       <c r="D675" s="1" t="s">
         <v>1727</v>
@@ -15937,10 +15943,10 @@
         <v>1726</v>
       </c>
       <c r="B676" t="s">
-        <v>1488</v>
+        <v>131</v>
       </c>
       <c r="C676" s="1" t="s">
-        <v>1488</v>
+        <v>131</v>
       </c>
       <c r="D676" s="1" t="s">
         <v>1727</v>
@@ -15951,10 +15957,10 @@
         <v>1726</v>
       </c>
       <c r="B677" t="s">
-        <v>1731</v>
+        <v>1730</v>
       </c>
       <c r="C677" s="1" t="s">
-        <v>1731</v>
+        <v>1730</v>
       </c>
       <c r="D677" s="1" t="s">
         <v>1727</v>
@@ -15965,10 +15971,10 @@
         <v>1726</v>
       </c>
       <c r="B678" t="s">
-        <v>1732</v>
+        <v>1488</v>
       </c>
       <c r="C678" s="1" t="s">
-        <v>1732</v>
+        <v>1488</v>
       </c>
       <c r="D678" s="1" t="s">
         <v>1727</v>
@@ -15979,10 +15985,10 @@
         <v>1726</v>
       </c>
       <c r="B679" t="s">
-        <v>1733</v>
+        <v>1731</v>
       </c>
       <c r="C679" s="1" t="s">
-        <v>1733</v>
+        <v>1731</v>
       </c>
       <c r="D679" s="1" t="s">
         <v>1727</v>
@@ -15993,10 +15999,10 @@
         <v>1726</v>
       </c>
       <c r="B680" t="s">
-        <v>1734</v>
+        <v>1732</v>
       </c>
       <c r="C680" s="1" t="s">
-        <v>1734</v>
+        <v>1732</v>
       </c>
       <c r="D680" s="1" t="s">
         <v>1727</v>
@@ -16007,10 +16013,10 @@
         <v>1726</v>
       </c>
       <c r="B681" t="s">
-        <v>1735</v>
+        <v>1733</v>
       </c>
       <c r="C681" s="1" t="s">
-        <v>1735</v>
+        <v>1733</v>
       </c>
       <c r="D681" s="1" t="s">
         <v>1727</v>
@@ -16021,10 +16027,10 @@
         <v>1726</v>
       </c>
       <c r="B682" t="s">
-        <v>1736</v>
+        <v>1734</v>
       </c>
       <c r="C682" s="1" t="s">
-        <v>1736</v>
+        <v>1734</v>
       </c>
       <c r="D682" s="1" t="s">
         <v>1727</v>
@@ -16035,10 +16041,10 @@
         <v>1726</v>
       </c>
       <c r="B683" t="s">
-        <v>1737</v>
+        <v>1735</v>
       </c>
       <c r="C683" s="1" t="s">
-        <v>1737</v>
+        <v>1735</v>
       </c>
       <c r="D683" s="1" t="s">
         <v>1727</v>
@@ -16049,10 +16055,10 @@
         <v>1726</v>
       </c>
       <c r="B684" t="s">
-        <v>1738</v>
+        <v>1736</v>
       </c>
       <c r="C684" s="1" t="s">
-        <v>1738</v>
+        <v>1736</v>
       </c>
       <c r="D684" s="1" t="s">
         <v>1727</v>
@@ -16063,10 +16069,10 @@
         <v>1726</v>
       </c>
       <c r="B685" t="s">
-        <v>1739</v>
+        <v>1737</v>
       </c>
       <c r="C685" s="1" t="s">
-        <v>1739</v>
+        <v>1737</v>
       </c>
       <c r="D685" s="1" t="s">
         <v>1727</v>
@@ -16074,30 +16080,30 @@
     </row>
     <row r="686" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A686" t="s">
-        <v>1740</v>
+        <v>1726</v>
       </c>
       <c r="B686" t="s">
-        <v>1741</v>
+        <v>1738</v>
       </c>
       <c r="C686" s="1" t="s">
-        <v>1741</v>
+        <v>1738</v>
       </c>
       <c r="D686" s="1" t="s">
-        <v>1742</v>
+        <v>1727</v>
       </c>
     </row>
     <row r="687" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A687" t="s">
-        <v>1740</v>
+        <v>1726</v>
       </c>
       <c r="B687" t="s">
-        <v>1743</v>
+        <v>1739</v>
       </c>
       <c r="C687" s="1" t="s">
-        <v>1743</v>
+        <v>1739</v>
       </c>
       <c r="D687" s="1" t="s">
-        <v>1742</v>
+        <v>1727</v>
       </c>
     </row>
     <row r="688" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -16105,10 +16111,10 @@
         <v>1740</v>
       </c>
       <c r="B688" t="s">
-        <v>1744</v>
+        <v>1741</v>
       </c>
       <c r="C688" s="1" t="s">
-        <v>1744</v>
+        <v>1741</v>
       </c>
       <c r="D688" s="1" t="s">
         <v>1742</v>
@@ -16119,10 +16125,10 @@
         <v>1740</v>
       </c>
       <c r="B689" t="s">
-        <v>1745</v>
+        <v>1743</v>
       </c>
       <c r="C689" s="1" t="s">
-        <v>1745</v>
+        <v>1743</v>
       </c>
       <c r="D689" s="1" t="s">
         <v>1742</v>
@@ -16130,86 +16136,86 @@
     </row>
     <row r="690" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A690" t="s">
-        <v>1746</v>
+        <v>1740</v>
       </c>
       <c r="B690" t="s">
-        <v>1747</v>
+        <v>1744</v>
       </c>
       <c r="C690" s="1" t="s">
-        <v>1747</v>
+        <v>1744</v>
       </c>
       <c r="D690" s="1" t="s">
-        <v>1748</v>
+        <v>1742</v>
       </c>
     </row>
     <row r="691" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A691" t="s">
+        <v>1740</v>
+      </c>
+      <c r="B691" t="s">
+        <v>1745</v>
+      </c>
+      <c r="C691" s="1" t="s">
+        <v>1745</v>
+      </c>
+      <c r="D691" s="1" t="s">
+        <v>1742</v>
+      </c>
+    </row>
+    <row r="692" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A692" t="s">
         <v>1746</v>
       </c>
-      <c r="B691" t="s">
+      <c r="B692" t="s">
+        <v>1747</v>
+      </c>
+      <c r="C692" s="1" t="s">
+        <v>1747</v>
+      </c>
+      <c r="D692" s="1" t="s">
+        <v>1748</v>
+      </c>
+    </row>
+    <row r="693" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A693" t="s">
+        <v>1746</v>
+      </c>
+      <c r="B693" t="s">
         <v>1749</v>
       </c>
-      <c r="C691" s="1" t="s">
+      <c r="C693" s="1" t="s">
         <v>1749</v>
       </c>
-      <c r="D691" s="1" t="s">
+      <c r="D693" s="1" t="s">
         <v>1748</v>
       </c>
     </row>
-    <row r="692" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A692" t="s">
+    <row r="694" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A694" t="s">
         <v>1750</v>
       </c>
-      <c r="B692" t="s">
+      <c r="B694" t="s">
         <v>1751</v>
       </c>
-      <c r="C692" s="1" t="s">
+      <c r="C694" s="1" t="s">
         <v>1751</v>
       </c>
-      <c r="D692" s="1" t="s">
+      <c r="D694" s="1" t="s">
         <v>1752</v>
       </c>
     </row>
-    <row r="693" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A693" t="s">
+    <row r="695" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A695" t="s">
         <v>1750</v>
       </c>
-      <c r="B693" t="s">
+      <c r="B695" t="s">
         <v>1753</v>
       </c>
-      <c r="C693" s="1" t="s">
+      <c r="C695" s="1" t="s">
         <v>1753</v>
       </c>
-      <c r="D693" s="1" t="s">
+      <c r="D695" s="1" t="s">
         <v>1752</v>
-      </c>
-    </row>
-    <row r="694" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A694" t="s">
-        <v>1754</v>
-      </c>
-      <c r="B694" t="s">
-        <v>1755</v>
-      </c>
-      <c r="C694" s="1" t="s">
-        <v>1755</v>
-      </c>
-      <c r="D694" s="1" t="s">
-        <v>1756</v>
-      </c>
-    </row>
-    <row r="695" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A695" t="s">
-        <v>1754</v>
-      </c>
-      <c r="B695" t="s">
-        <v>1757</v>
-      </c>
-      <c r="C695" s="1" t="s">
-        <v>1757</v>
-      </c>
-      <c r="D695" s="1" t="s">
-        <v>1756</v>
       </c>
     </row>
     <row r="696" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -16217,10 +16223,10 @@
         <v>1754</v>
       </c>
       <c r="B696" t="s">
-        <v>1758</v>
+        <v>1755</v>
       </c>
       <c r="C696" s="1" t="s">
-        <v>1758</v>
+        <v>1755</v>
       </c>
       <c r="D696" s="1" t="s">
         <v>1756</v>
@@ -16231,10 +16237,10 @@
         <v>1754</v>
       </c>
       <c r="B697" t="s">
-        <v>1759</v>
+        <v>1757</v>
       </c>
       <c r="C697" s="1" t="s">
-        <v>1759</v>
+        <v>1757</v>
       </c>
       <c r="D697" s="1" t="s">
         <v>1756</v>
@@ -16245,10 +16251,10 @@
         <v>1754</v>
       </c>
       <c r="B698" t="s">
-        <v>1760</v>
+        <v>1758</v>
       </c>
       <c r="C698" s="1" t="s">
-        <v>1760</v>
+        <v>1758</v>
       </c>
       <c r="D698" s="1" t="s">
         <v>1756</v>
@@ -16259,10 +16265,10 @@
         <v>1754</v>
       </c>
       <c r="B699" t="s">
-        <v>1761</v>
+        <v>1759</v>
       </c>
       <c r="C699" s="1" t="s">
-        <v>1761</v>
+        <v>1759</v>
       </c>
       <c r="D699" s="1" t="s">
         <v>1756</v>
@@ -16273,10 +16279,10 @@
         <v>1754</v>
       </c>
       <c r="B700" t="s">
-        <v>1762</v>
+        <v>1760</v>
       </c>
       <c r="C700" s="1" t="s">
-        <v>1762</v>
+        <v>1760</v>
       </c>
       <c r="D700" s="1" t="s">
         <v>1756</v>
@@ -16284,30 +16290,30 @@
     </row>
     <row r="701" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A701" t="s">
-        <v>1763</v>
+        <v>1754</v>
       </c>
       <c r="B701" t="s">
-        <v>1764</v>
+        <v>1761</v>
       </c>
       <c r="C701" s="1" t="s">
-        <v>1765</v>
+        <v>1761</v>
       </c>
       <c r="D701" s="1" t="s">
-        <v>1766</v>
+        <v>1756</v>
       </c>
     </row>
     <row r="702" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A702" t="s">
-        <v>1763</v>
+        <v>1754</v>
       </c>
       <c r="B702" t="s">
-        <v>1767</v>
+        <v>1762</v>
       </c>
       <c r="C702" s="1" t="s">
-        <v>1768</v>
+        <v>1762</v>
       </c>
       <c r="D702" s="1" t="s">
-        <v>1769</v>
+        <v>1756</v>
       </c>
     </row>
     <row r="703" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -16315,41 +16321,41 @@
         <v>1763</v>
       </c>
       <c r="B703" t="s">
-        <v>1770</v>
+        <v>1764</v>
       </c>
       <c r="C703" s="1" t="s">
-        <v>1771</v>
+        <v>1765</v>
       </c>
       <c r="D703" s="1" t="s">
-        <v>1772</v>
+        <v>1766</v>
       </c>
     </row>
     <row r="704" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A704" t="s">
-        <v>1773</v>
+        <v>1763</v>
       </c>
       <c r="B704" t="s">
-        <v>1774</v>
+        <v>1767</v>
       </c>
       <c r="C704" s="1" t="s">
-        <v>1654</v>
+        <v>1768</v>
       </c>
       <c r="D704" s="1" t="s">
-        <v>1775</v>
+        <v>1769</v>
       </c>
     </row>
     <row r="705" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A705" t="s">
-        <v>1773</v>
+        <v>1763</v>
       </c>
       <c r="B705" t="s">
-        <v>1776</v>
+        <v>1770</v>
       </c>
       <c r="C705" s="1" t="s">
-        <v>1656</v>
+        <v>1771</v>
       </c>
       <c r="D705" s="1" t="s">
-        <v>1777</v>
+        <v>1772</v>
       </c>
     </row>
     <row r="706" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -16357,83 +16363,83 @@
         <v>1773</v>
       </c>
       <c r="B706" t="s">
-        <v>1778</v>
+        <v>1774</v>
       </c>
       <c r="C706" s="1" t="s">
-        <v>1779</v>
+        <v>1654</v>
       </c>
       <c r="D706" s="1" t="s">
-        <v>1780</v>
+        <v>1775</v>
       </c>
     </row>
     <row r="707" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A707" t="s">
-        <v>1781</v>
+        <v>1773</v>
       </c>
       <c r="B707" t="s">
-        <v>1782</v>
+        <v>1776</v>
       </c>
       <c r="C707" s="1" t="s">
-        <v>1782</v>
+        <v>1656</v>
       </c>
       <c r="D707" s="1" t="s">
-        <v>1783</v>
+        <v>1777</v>
       </c>
     </row>
     <row r="708" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A708" t="s">
-        <v>1781</v>
+        <v>1773</v>
       </c>
       <c r="B708" t="s">
-        <v>1784</v>
+        <v>1778</v>
       </c>
       <c r="C708" s="1" t="s">
-        <v>1784</v>
+        <v>1779</v>
       </c>
       <c r="D708" s="1" t="s">
-        <v>1783</v>
+        <v>1780</v>
       </c>
     </row>
     <row r="709" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A709" t="s">
-        <v>1785</v>
+        <v>1781</v>
       </c>
       <c r="B709" t="s">
-        <v>1786</v>
+        <v>1782</v>
       </c>
       <c r="C709" s="1" t="s">
-        <v>1786</v>
+        <v>1782</v>
       </c>
       <c r="D709" s="1" t="s">
-        <v>1787</v>
+        <v>1783</v>
       </c>
     </row>
     <row r="710" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A710" t="s">
-        <v>1788</v>
+        <v>1781</v>
       </c>
       <c r="B710" t="s">
-        <v>1789</v>
+        <v>1784</v>
       </c>
       <c r="C710" s="1" t="s">
-        <v>1789</v>
+        <v>1784</v>
       </c>
       <c r="D710" s="1" t="s">
-        <v>1790</v>
+        <v>1783</v>
       </c>
     </row>
     <row r="711" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A711" t="s">
-        <v>1788</v>
+        <v>1785</v>
       </c>
       <c r="B711" t="s">
-        <v>1791</v>
+        <v>1786</v>
       </c>
       <c r="C711" s="1" t="s">
-        <v>1791</v>
+        <v>1786</v>
       </c>
       <c r="D711" s="1" t="s">
-        <v>1790</v>
+        <v>1787</v>
       </c>
     </row>
     <row r="712" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -16441,40 +16447,68 @@
         <v>1788</v>
       </c>
       <c r="B712" t="s">
-        <v>1792</v>
+        <v>1789</v>
       </c>
       <c r="C712" s="1" t="s">
-        <v>1792</v>
+        <v>1789</v>
       </c>
       <c r="D712" s="1" t="s">
         <v>1790</v>
       </c>
     </row>
-    <row r="713" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="713" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A713" t="s">
+        <v>1788</v>
+      </c>
+      <c r="B713" t="s">
+        <v>1791</v>
+      </c>
+      <c r="C713" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="D713" s="1" t="s">
+        <v>1790</v>
+      </c>
+    </row>
+    <row r="714" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A714" t="s">
+        <v>1788</v>
+      </c>
+      <c r="B714" t="s">
+        <v>1792</v>
+      </c>
+      <c r="C714" s="1" t="s">
+        <v>1792</v>
+      </c>
+      <c r="D714" s="1" t="s">
+        <v>1790</v>
+      </c>
+    </row>
+    <row r="715" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A715" t="s">
         <v>1793</v>
       </c>
-      <c r="B713" t="s">
+      <c r="B715" t="s">
         <v>1794</v>
       </c>
-      <c r="C713" s="1" t="s">
+      <c r="C715" s="1" t="s">
         <v>1794</v>
       </c>
-      <c r="D713" s="1" t="s">
+      <c r="D715" s="1" t="s">
         <v>1795</v>
       </c>
     </row>
-    <row r="714" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A714" t="s">
+    <row r="716" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A716" t="s">
         <v>1793</v>
       </c>
-      <c r="B714" t="s">
+      <c r="B716" t="s">
         <v>1796</v>
       </c>
-      <c r="C714" s="1" t="s">
+      <c r="C716" s="1" t="s">
         <v>1796</v>
       </c>
-      <c r="D714" s="1" t="s">
+      <c r="D716" s="1" t="s">
         <v>1795</v>
       </c>
     </row>

</xml_diff>